<commit_message>
Updating Fulldata.xls with new observations (last tab)!
</commit_message>
<xml_diff>
--- a/mobley/mnsol/Fulldata.xlsx
+++ b/mobley/mnsol/Fulldata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="1180" windowWidth="24960" windowHeight="13900" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="220" yWindow="1180" windowWidth="24960" windowHeight="13900" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Solvents_neutral&amp;ions" sheetId="3" r:id="rId3"/>
     <sheet name="Solvents_ions_only" sheetId="4" r:id="rId4"/>
     <sheet name="consistent_set_neutral+ions" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13186" uniqueCount="583">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13218" uniqueCount="615">
   <si>
     <t>Compound</t>
   </si>
@@ -1781,12 +1782,108 @@
   <si>
     <t>count</t>
   </si>
+  <si>
+    <t>Nonpolar</t>
+  </si>
+  <si>
+    <t>Polar</t>
+  </si>
+  <si>
+    <t>Ions</t>
+  </si>
+  <si>
+    <t>Neutral species</t>
+  </si>
+  <si>
+    <t>Solvent</t>
+  </si>
+  <si>
+    <t>alpha</t>
+  </si>
+  <si>
+    <t>beta</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>mu</t>
+  </si>
+  <si>
+    <t>phi</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>RMS</t>
+  </si>
+  <si>
+    <t>Dipole moment</t>
+  </si>
+  <si>
+    <t>eps</t>
+  </si>
+  <si>
+    <t>'Water'</t>
+  </si>
+  <si>
+    <t>Hydrogen bond?</t>
+  </si>
+  <si>
+    <t>'Octanol'</t>
+  </si>
+  <si>
+    <t>~=2 surface area offset</t>
+  </si>
+  <si>
+    <t>'Dichloroethane'</t>
+  </si>
+  <si>
+    <t>High RMS for NP solvent</t>
+  </si>
+  <si>
+    <t>'Propanone'</t>
+  </si>
+  <si>
+    <t>small mu</t>
+  </si>
+  <si>
+    <t>'Dimethylsulfoxide'</t>
+  </si>
+  <si>
+    <t>Polar solvents</t>
+  </si>
+  <si>
+    <t>'Propanol'</t>
+  </si>
+  <si>
+    <t>Nonpolar solvents</t>
+  </si>
+  <si>
+    <t>'Dimethylformamide'</t>
+  </si>
+  <si>
+    <t>'Ethanol'</t>
+  </si>
+  <si>
+    <t>'Methanol'</t>
+  </si>
+  <si>
+    <t>'Acetonitrile'</t>
+  </si>
+  <si>
+    <t>geometry</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1817,8 +1914,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1839,13 +1941,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.249977111117893"/>
+        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1859,7 +1985,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1871,8 +1997,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1888,22 +2018,44 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1914,6 +2066,451 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1099457</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="42" name="Picture 41"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10299700" y="482600"/>
+          <a:ext cx="807357" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1003300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>752143</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10375900" y="2857500"/>
+          <a:ext cx="635000" cy="701343"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>55154</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>993775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>698500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="44" name="Picture 43"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10375900" y="2112554"/>
+          <a:ext cx="625475" cy="643346"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1056975</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>774700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10287000" y="4368800"/>
+          <a:ext cx="777575" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1308100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>488898</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10071100" y="6591300"/>
+          <a:ext cx="1244600" cy="323798"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1274646</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>546100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="5918200"/>
+          <a:ext cx="1185746" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1333500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>495299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10033000" y="5290050"/>
+          <a:ext cx="1308100" cy="361449"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>163688</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1346200</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>495299</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10020300" y="3897488"/>
+          <a:ext cx="1333500" cy="331611"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>39851</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1143000</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>711200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10223500" y="1513051"/>
+          <a:ext cx="927100" cy="671349"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1287616</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>482600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Picture 50"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10045700" y="1003300"/>
+          <a:ext cx="1249516" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2181,8 +2778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CV514"/>
   <sheetViews>
-    <sheetView topLeftCell="CJ1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A508" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="CL1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A498" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="CU2" sqref="CU2:CV513"/>
     </sheetView>
   </sheetViews>
@@ -2569,11 +3166,11 @@
         <v>1</v>
       </c>
       <c r="CU2" t="str">
-        <f>IF(ISNUMBER(CK2),A2,"")</f>
+        <f>IF(ISNUMBER(CD2),A2,"")</f>
         <v/>
       </c>
       <c r="CV2" t="str">
-        <f>IF(ISNUMBER(CK2),CK2,"")</f>
+        <f>IF(ISNUMBER(CD2),CD2,"")</f>
         <v/>
       </c>
     </row>
@@ -2658,11 +3255,11 @@
         <v>1</v>
       </c>
       <c r="CU3" t="str">
-        <f t="shared" ref="CU3:CU66" si="0">IF(ISNUMBER(CK3),A3,"")</f>
+        <f t="shared" ref="CU3:CU66" si="0">IF(ISNUMBER(CD3),A3,"")</f>
         <v/>
       </c>
       <c r="CV3" t="str">
-        <f t="shared" ref="CV3:CV66" si="1">IF(ISNUMBER(CK3),CK3,"")</f>
+        <f t="shared" ref="CV3:CV66" si="1">IF(ISNUMBER(CD3),CD3,"")</f>
         <v/>
       </c>
     </row>
@@ -2754,11 +3351,11 @@
       </c>
       <c r="CU4" t="str">
         <f t="shared" si="0"/>
-        <v>1_bromobutane</v>
-      </c>
-      <c r="CV4">
+        <v/>
+      </c>
+      <c r="CV4" t="str">
         <f t="shared" si="1"/>
-        <v>-4.16</v>
+        <v/>
       </c>
     </row>
     <row r="5" spans="1:100" x14ac:dyDescent="0.2">
@@ -3116,11 +3713,11 @@
       </c>
       <c r="CU8" t="str">
         <f t="shared" si="0"/>
-        <v>1_bromopentane</v>
-      </c>
-      <c r="CV8">
+        <v/>
+      </c>
+      <c r="CV8" t="str">
         <f t="shared" si="1"/>
-        <v>-4.68</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:100" x14ac:dyDescent="0.2">
@@ -3211,11 +3808,11 @@
       </c>
       <c r="CU9" t="str">
         <f t="shared" si="0"/>
-        <v>1_bromopropane</v>
-      </c>
-      <c r="CV9">
+        <v/>
+      </c>
+      <c r="CV9" t="str">
         <f t="shared" si="1"/>
-        <v>-3.42</v>
+        <v/>
       </c>
     </row>
     <row r="10" spans="1:100" x14ac:dyDescent="0.2">
@@ -3757,11 +4354,11 @@
       </c>
       <c r="CU15" t="str">
         <f t="shared" si="0"/>
-        <v>1_chloropropane</v>
-      </c>
-      <c r="CV15">
+        <v/>
+      </c>
+      <c r="CV15" t="str">
         <f t="shared" si="1"/>
-        <v>-3.06</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:100" x14ac:dyDescent="0.2">
@@ -3941,11 +4538,11 @@
       </c>
       <c r="CU17" t="str">
         <f t="shared" si="0"/>
-        <v>1_iodobutane</v>
-      </c>
-      <c r="CV17">
+        <v/>
+      </c>
+      <c r="CV17" t="str">
         <f t="shared" si="1"/>
-        <v>-4.4400000000000004</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:100" x14ac:dyDescent="0.2">
@@ -4306,11 +4903,11 @@
       </c>
       <c r="CU21" t="str">
         <f t="shared" si="0"/>
-        <v>1_iodopropane</v>
-      </c>
-      <c r="CV21">
+        <v/>
+      </c>
+      <c r="CV21" t="str">
         <f t="shared" si="1"/>
-        <v>-3.99</v>
+        <v/>
       </c>
     </row>
     <row r="22" spans="1:100" x14ac:dyDescent="0.2">
@@ -4858,11 +5455,11 @@
       </c>
       <c r="CU27" t="str">
         <f t="shared" si="0"/>
-        <v>1_naphthylamine</v>
-      </c>
-      <c r="CV27">
+        <v/>
+      </c>
+      <c r="CV27" t="str">
         <f t="shared" si="1"/>
-        <v>-10.34</v>
+        <v/>
       </c>
     </row>
     <row r="28" spans="1:100" x14ac:dyDescent="0.2">
@@ -4956,11 +5553,11 @@
       </c>
       <c r="CU28" t="str">
         <f t="shared" si="0"/>
-        <v>1_nitrobutane</v>
-      </c>
-      <c r="CV28">
+        <v/>
+      </c>
+      <c r="CV28" t="str">
         <f t="shared" si="1"/>
-        <v>-5.1100000000000003</v>
+        <v/>
       </c>
     </row>
     <row r="29" spans="1:100" x14ac:dyDescent="0.2">
@@ -5152,11 +5749,11 @@
       </c>
       <c r="CU30" t="str">
         <f t="shared" si="0"/>
-        <v>1_nitropropane</v>
-      </c>
-      <c r="CV30">
+        <v/>
+      </c>
+      <c r="CV30" t="str">
         <f t="shared" si="1"/>
-        <v>-4.4400000000000004</v>
+        <v/>
       </c>
     </row>
     <row r="31" spans="1:100" x14ac:dyDescent="0.2">
@@ -5603,11 +6200,11 @@
       </c>
       <c r="CU35" t="str">
         <f t="shared" si="0"/>
-        <v>11_difluoroethane</v>
-      </c>
-      <c r="CV35">
+        <v/>
+      </c>
+      <c r="CV35" t="str">
         <f t="shared" si="1"/>
-        <v>-1.1299999999999999</v>
+        <v/>
       </c>
     </row>
     <row r="36" spans="1:100" x14ac:dyDescent="0.2">
@@ -5701,11 +6298,11 @@
       </c>
       <c r="CU36" t="str">
         <f t="shared" si="0"/>
-        <v>111_trichloroethane</v>
-      </c>
-      <c r="CV36">
+        <v/>
+      </c>
+      <c r="CV36" t="str">
         <f t="shared" si="1"/>
-        <v>-3.69</v>
+        <v/>
       </c>
     </row>
     <row r="37" spans="1:100" x14ac:dyDescent="0.2">
@@ -5882,11 +6479,11 @@
       </c>
       <c r="CU38" t="str">
         <f t="shared" si="0"/>
-        <v>111_trifluoropropan_2_ol</v>
-      </c>
-      <c r="CV38">
+        <v/>
+      </c>
+      <c r="CV38" t="str">
         <f t="shared" si="1"/>
-        <v>-5.12</v>
+        <v/>
       </c>
     </row>
     <row r="39" spans="1:100" x14ac:dyDescent="0.2">
@@ -6155,11 +6752,11 @@
       </c>
       <c r="CU41" t="str">
         <f t="shared" si="0"/>
-        <v>112_trichloro_122_trifluoroethane</v>
-      </c>
-      <c r="CV41">
+        <v/>
+      </c>
+      <c r="CV41" t="str">
         <f t="shared" si="1"/>
-        <v>-2.54</v>
+        <v/>
       </c>
     </row>
     <row r="42" spans="1:100" x14ac:dyDescent="0.2">
@@ -6250,11 +6847,11 @@
       </c>
       <c r="CU42" t="str">
         <f t="shared" si="0"/>
-        <v>112_trichloroethane</v>
-      </c>
-      <c r="CV42">
+        <v/>
+      </c>
+      <c r="CV42" t="str">
         <f t="shared" si="1"/>
-        <v>-4.53</v>
+        <v/>
       </c>
     </row>
     <row r="43" spans="1:100" x14ac:dyDescent="0.2">
@@ -6615,11 +7212,11 @@
       </c>
       <c r="CU46" t="str">
         <f t="shared" si="0"/>
-        <v>12_dichlorobenzene</v>
-      </c>
-      <c r="CV46">
+        <v/>
+      </c>
+      <c r="CV46" t="str">
         <f t="shared" si="1"/>
-        <v>-6.01</v>
+        <v/>
       </c>
     </row>
     <row r="47" spans="1:100" x14ac:dyDescent="0.2">
@@ -6719,11 +7316,11 @@
       </c>
       <c r="CU47" t="str">
         <f t="shared" si="0"/>
-        <v>12_dichloroethane</v>
-      </c>
-      <c r="CV47">
+        <v/>
+      </c>
+      <c r="CV47" t="str">
         <f t="shared" si="1"/>
-        <v>-3.81</v>
+        <v/>
       </c>
     </row>
     <row r="48" spans="1:100" x14ac:dyDescent="0.2">
@@ -6992,11 +7589,11 @@
       </c>
       <c r="CU50" t="str">
         <f t="shared" si="0"/>
-        <v>12_dimethoxyethane</v>
-      </c>
-      <c r="CV50">
+        <v/>
+      </c>
+      <c r="CV50" t="str">
         <f t="shared" si="1"/>
-        <v>-4.55</v>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:100" x14ac:dyDescent="0.2">
@@ -7102,11 +7699,11 @@
       </c>
       <c r="CU51" t="str">
         <f t="shared" si="0"/>
-        <v>12_ethanediol</v>
-      </c>
-      <c r="CV51">
+        <v/>
+      </c>
+      <c r="CV51" t="str">
         <f t="shared" si="1"/>
-        <v>-7.44</v>
+        <v/>
       </c>
     </row>
     <row r="52" spans="1:100" x14ac:dyDescent="0.2">
@@ -7728,11 +8325,11 @@
       </c>
       <c r="CU58" t="str">
         <f t="shared" si="0"/>
-        <v>1245_tetrachlorobenzene</v>
-      </c>
-      <c r="CV58">
+        <v/>
+      </c>
+      <c r="CV58" t="str">
         <f t="shared" si="1"/>
-        <v>-7.61</v>
+        <v/>
       </c>
     </row>
     <row r="59" spans="1:100" x14ac:dyDescent="0.2">
@@ -8296,7 +8893,7 @@
       </c>
       <c r="CV64">
         <f t="shared" si="1"/>
-        <v>-5.67</v>
+        <v>-7.75</v>
       </c>
     </row>
     <row r="65" spans="1:100" x14ac:dyDescent="0.2">
@@ -8558,11 +9155,11 @@
         <v>1</v>
       </c>
       <c r="CU67" t="str">
-        <f t="shared" ref="CU67:CU130" si="4">IF(ISNUMBER(CK67),A67,"")</f>
+        <f t="shared" ref="CU67:CU130" si="4">IF(ISNUMBER(CD67),A67,"")</f>
         <v/>
       </c>
       <c r="CV67" t="str">
-        <f t="shared" ref="CV67:CV130" si="5">IF(ISNUMBER(CK67),CK67,"")</f>
+        <f t="shared" ref="CV67:CV130" si="5">IF(ISNUMBER(CD67),CD67,"")</f>
         <v/>
       </c>
     </row>
@@ -8775,7 +9372,7 @@
       </c>
       <c r="CV68">
         <f t="shared" si="5"/>
-        <v>-4.8899999999999997</v>
+        <v>-5.03</v>
       </c>
     </row>
     <row r="69" spans="1:100" x14ac:dyDescent="0.2">
@@ -8955,11 +9552,11 @@
       </c>
       <c r="CU70" t="str">
         <f t="shared" si="4"/>
-        <v>2_bromopropane</v>
-      </c>
-      <c r="CV70">
+        <v/>
+      </c>
+      <c r="CV70" t="str">
         <f t="shared" si="5"/>
-        <v>-3.4</v>
+        <v/>
       </c>
     </row>
     <row r="71" spans="1:100" x14ac:dyDescent="0.2">
@@ -9516,11 +10113,11 @@
       </c>
       <c r="CU76" t="str">
         <f t="shared" si="4"/>
-        <v>2_chlorophenol</v>
-      </c>
-      <c r="CV76">
+        <v/>
+      </c>
+      <c r="CV76" t="str">
         <f t="shared" si="5"/>
-        <v>-7.48</v>
+        <v/>
       </c>
     </row>
     <row r="77" spans="1:100" x14ac:dyDescent="0.2">
@@ -9611,11 +10208,11 @@
       </c>
       <c r="CU77" t="str">
         <f t="shared" si="4"/>
-        <v>2_chloropropane</v>
-      </c>
-      <c r="CV77">
+        <v/>
+      </c>
+      <c r="CV77" t="str">
         <f t="shared" si="5"/>
-        <v>-2.84</v>
+        <v/>
       </c>
     </row>
     <row r="78" spans="1:100" x14ac:dyDescent="0.2">
@@ -9792,11 +10389,11 @@
       </c>
       <c r="CU79" t="str">
         <f t="shared" si="4"/>
-        <v>2_chlorotoluene</v>
-      </c>
-      <c r="CV79">
+        <v/>
+      </c>
+      <c r="CV79" t="str">
         <f t="shared" si="5"/>
-        <v>-5.8</v>
+        <v/>
       </c>
     </row>
     <row r="80" spans="1:100" x14ac:dyDescent="0.2">
@@ -9976,11 +10573,11 @@
       </c>
       <c r="CU81" t="str">
         <f t="shared" si="4"/>
-        <v>2_ethylpyrazine</v>
-      </c>
-      <c r="CV81">
+        <v/>
+      </c>
+      <c r="CV81" t="str">
         <f t="shared" si="5"/>
-        <v>-6.4</v>
+        <v/>
       </c>
     </row>
     <row r="82" spans="1:100" x14ac:dyDescent="0.2">
@@ -10249,11 +10846,11 @@
       </c>
       <c r="CU84" t="str">
         <f t="shared" si="4"/>
-        <v>2_fluorophenol</v>
-      </c>
-      <c r="CV84">
+        <v/>
+      </c>
+      <c r="CV84" t="str">
         <f t="shared" si="5"/>
-        <v>-7.62</v>
+        <v/>
       </c>
     </row>
     <row r="85" spans="1:100" x14ac:dyDescent="0.2">
@@ -10350,11 +10947,11 @@
       </c>
       <c r="CU85" t="str">
         <f t="shared" si="4"/>
-        <v>2_iodophenol</v>
-      </c>
-      <c r="CV85">
+        <v/>
+      </c>
+      <c r="CV85" t="str">
         <f t="shared" si="5"/>
-        <v>-9.81</v>
+        <v/>
       </c>
     </row>
     <row r="86" spans="1:100" x14ac:dyDescent="0.2">
@@ -10442,11 +11039,11 @@
       </c>
       <c r="CU86" t="str">
         <f t="shared" si="4"/>
-        <v>2_iodopropane</v>
-      </c>
-      <c r="CV86">
+        <v/>
+      </c>
+      <c r="CV86" t="str">
         <f t="shared" si="5"/>
-        <v>-4.4000000000000004</v>
+        <v/>
       </c>
     </row>
     <row r="87" spans="1:100" x14ac:dyDescent="0.2">
@@ -10896,11 +11493,11 @@
       </c>
       <c r="CU91" t="str">
         <f t="shared" si="4"/>
-        <v>2_methoxyethanol</v>
-      </c>
-      <c r="CV91">
+        <v/>
+      </c>
+      <c r="CV91" t="str">
         <f t="shared" si="5"/>
-        <v>-5.83</v>
+        <v/>
       </c>
     </row>
     <row r="92" spans="1:100" x14ac:dyDescent="0.2">
@@ -12160,11 +12757,11 @@
       </c>
       <c r="CU105" t="str">
         <f t="shared" si="4"/>
-        <v>2_methylpropan_2_ol</v>
-      </c>
-      <c r="CV105">
+        <v/>
+      </c>
+      <c r="CV105" t="str">
         <f t="shared" si="5"/>
-        <v>-4.78</v>
+        <v/>
       </c>
     </row>
     <row r="106" spans="1:100" x14ac:dyDescent="0.2">
@@ -12255,11 +12852,11 @@
       </c>
       <c r="CU106" t="str">
         <f t="shared" si="4"/>
-        <v>2_methylpropane</v>
-      </c>
-      <c r="CV106">
+        <v/>
+      </c>
+      <c r="CV106" t="str">
         <f t="shared" si="5"/>
-        <v>-1.45</v>
+        <v/>
       </c>
     </row>
     <row r="107" spans="1:100" x14ac:dyDescent="0.2">
@@ -12350,11 +12947,11 @@
       </c>
       <c r="CU107" t="str">
         <f t="shared" si="4"/>
-        <v>2_methylpropene</v>
-      </c>
-      <c r="CV107">
+        <v/>
+      </c>
+      <c r="CV107" t="str">
         <f t="shared" si="5"/>
-        <v>-2.0299999999999998</v>
+        <v/>
       </c>
     </row>
     <row r="108" spans="1:100" x14ac:dyDescent="0.2">
@@ -12445,11 +13042,11 @@
       </c>
       <c r="CU108" t="str">
         <f t="shared" si="4"/>
-        <v>2_methylpyrazine</v>
-      </c>
-      <c r="CV108">
+        <v/>
+      </c>
+      <c r="CV108" t="str">
         <f t="shared" si="5"/>
-        <v>-5.87</v>
+        <v/>
       </c>
     </row>
     <row r="109" spans="1:100" x14ac:dyDescent="0.2">
@@ -12552,11 +13149,11 @@
       </c>
       <c r="CU109" t="str">
         <f t="shared" si="4"/>
-        <v>2_methylpyridine</v>
-      </c>
-      <c r="CV109">
+        <v/>
+      </c>
+      <c r="CV109" t="str">
         <f t="shared" si="5"/>
-        <v>-6.14</v>
+        <v/>
       </c>
     </row>
     <row r="110" spans="1:100" x14ac:dyDescent="0.2">
@@ -12852,11 +13449,11 @@
       </c>
       <c r="CU112" t="str">
         <f t="shared" si="4"/>
-        <v>2_naphthol</v>
-      </c>
-      <c r="CV112">
+        <v/>
+      </c>
+      <c r="CV112" t="str">
         <f t="shared" si="5"/>
-        <v>-11.78</v>
+        <v/>
       </c>
     </row>
     <row r="113" spans="1:100" x14ac:dyDescent="0.2">
@@ -12962,11 +13559,11 @@
       </c>
       <c r="CU113" t="str">
         <f t="shared" si="4"/>
-        <v>2_naphthylamine</v>
-      </c>
-      <c r="CV113">
+        <v/>
+      </c>
+      <c r="CV113" t="str">
         <f t="shared" si="5"/>
-        <v>-10.57</v>
+        <v/>
       </c>
     </row>
     <row r="114" spans="1:100" x14ac:dyDescent="0.2">
@@ -13235,11 +13832,11 @@
       </c>
       <c r="CU116" t="str">
         <f t="shared" si="4"/>
-        <v>2_nitropropane</v>
-      </c>
-      <c r="CV116">
+        <v/>
+      </c>
+      <c r="CV116" t="str">
         <f t="shared" si="5"/>
-        <v>-4.2300000000000004</v>
+        <v/>
       </c>
     </row>
     <row r="117" spans="1:100" x14ac:dyDescent="0.2">
@@ -13775,11 +14372,11 @@
       </c>
       <c r="CU122" t="str">
         <f t="shared" si="4"/>
-        <v>22_dimethylpropane</v>
-      </c>
-      <c r="CV122">
+        <v/>
+      </c>
+      <c r="CV122" t="str">
         <f t="shared" si="5"/>
-        <v>-1.74</v>
+        <v/>
       </c>
     </row>
     <row r="123" spans="1:100" x14ac:dyDescent="0.2">
@@ -13883,7 +14480,7 @@
       </c>
       <c r="CV123">
         <f t="shared" si="5"/>
-        <v>-4.8099999999999996</v>
+        <v>-6.93</v>
       </c>
     </row>
     <row r="124" spans="1:100" x14ac:dyDescent="0.2">
@@ -14590,11 +15187,11 @@
         <v>1</v>
       </c>
       <c r="CU131" t="str">
-        <f t="shared" ref="CU131:CU194" si="7">IF(ISNUMBER(CK131),A131,"")</f>
+        <f t="shared" ref="CU131:CU194" si="7">IF(ISNUMBER(CD131),A131,"")</f>
         <v/>
       </c>
       <c r="CV131" t="str">
-        <f t="shared" ref="CV131:CV194" si="8">IF(ISNUMBER(CK131),CK131,"")</f>
+        <f t="shared" ref="CV131:CV194" si="8">IF(ISNUMBER(CD131),CD131,"")</f>
         <v/>
       </c>
     </row>
@@ -15968,11 +16565,11 @@
       </c>
       <c r="CU146" t="str">
         <f t="shared" si="7"/>
-        <v>3_chlorophenol</v>
-      </c>
-      <c r="CV146">
+        <v/>
+      </c>
+      <c r="CV146" t="str">
         <f t="shared" si="8"/>
-        <v>-10.02</v>
+        <v/>
       </c>
     </row>
     <row r="147" spans="1:100" x14ac:dyDescent="0.2">
@@ -16149,11 +16746,11 @@
       </c>
       <c r="CU148" t="str">
         <f t="shared" si="7"/>
-        <v>3_chloropyridine</v>
-      </c>
-      <c r="CV148">
+        <v/>
+      </c>
+      <c r="CV148" t="str">
         <f t="shared" si="8"/>
-        <v>-5.82</v>
+        <v/>
       </c>
     </row>
     <row r="149" spans="1:100" x14ac:dyDescent="0.2">
@@ -17769,11 +18366,11 @@
       </c>
       <c r="CU166" t="str">
         <f t="shared" si="7"/>
-        <v>3_methylpyridine</v>
-      </c>
-      <c r="CV166">
+        <v/>
+      </c>
+      <c r="CV166" t="str">
         <f t="shared" si="8"/>
-        <v>-6.4</v>
+        <v/>
       </c>
     </row>
     <row r="167" spans="1:100" x14ac:dyDescent="0.2">
@@ -17870,11 +18467,11 @@
       </c>
       <c r="CU167" t="str">
         <f t="shared" si="7"/>
-        <v>3_nitroaniline</v>
-      </c>
-      <c r="CV167">
+        <v/>
+      </c>
+      <c r="CV167" t="str">
         <f t="shared" si="8"/>
-        <v>-10.71</v>
+        <v/>
       </c>
     </row>
     <row r="168" spans="1:100" x14ac:dyDescent="0.2">
@@ -17983,11 +18580,11 @@
       </c>
       <c r="CU168" t="str">
         <f t="shared" si="7"/>
-        <v>3_nitrophenol</v>
-      </c>
-      <c r="CV168">
+        <v/>
+      </c>
+      <c r="CV168" t="str">
         <f t="shared" si="8"/>
-        <v>-12.34</v>
+        <v/>
       </c>
     </row>
     <row r="169" spans="1:100" x14ac:dyDescent="0.2">
@@ -18295,11 +18892,11 @@
       </c>
       <c r="CU171" t="str">
         <f t="shared" si="7"/>
-        <v>33_dimethylbutan_2_one</v>
-      </c>
-      <c r="CV171">
+        <v/>
+      </c>
+      <c r="CV171" t="str">
         <f t="shared" si="8"/>
-        <v>-4.53</v>
+        <v/>
       </c>
     </row>
     <row r="172" spans="1:100" x14ac:dyDescent="0.2">
@@ -19079,11 +19676,11 @@
       </c>
       <c r="CU179" t="str">
         <f t="shared" si="7"/>
-        <v>4_bromophenol</v>
-      </c>
-      <c r="CV179">
+        <v/>
+      </c>
+      <c r="CV179" t="str">
         <f t="shared" si="8"/>
-        <v>-10.59</v>
+        <v/>
       </c>
     </row>
     <row r="180" spans="1:100" x14ac:dyDescent="0.2">
@@ -19174,11 +19771,11 @@
       </c>
       <c r="CU180" t="str">
         <f t="shared" si="7"/>
-        <v>4_bromotoluene</v>
-      </c>
-      <c r="CV180">
+        <v/>
+      </c>
+      <c r="CV180" t="str">
         <f t="shared" si="8"/>
-        <v>-6.16</v>
+        <v/>
       </c>
     </row>
     <row r="181" spans="1:100" x14ac:dyDescent="0.2">
@@ -19471,11 +20068,11 @@
       </c>
       <c r="CU183" t="str">
         <f t="shared" si="7"/>
-        <v>4_chlorophenol</v>
-      </c>
-      <c r="CV183">
+        <v/>
+      </c>
+      <c r="CV183" t="str">
         <f t="shared" si="8"/>
-        <v>-10.3</v>
+        <v/>
       </c>
     </row>
     <row r="184" spans="1:100" x14ac:dyDescent="0.2">
@@ -19833,11 +20430,11 @@
       </c>
       <c r="CU187" t="str">
         <f t="shared" si="7"/>
-        <v>4_ethylpyridine</v>
-      </c>
-      <c r="CV187">
+        <v/>
+      </c>
+      <c r="CV187" t="str">
         <f t="shared" si="8"/>
-        <v>-7.8</v>
+        <v/>
       </c>
     </row>
     <row r="188" spans="1:100" x14ac:dyDescent="0.2">
@@ -20023,11 +20620,11 @@
       </c>
       <c r="CU189" t="str">
         <f t="shared" si="7"/>
-        <v>4_fluorophenol</v>
-      </c>
-      <c r="CV189">
+        <v/>
+      </c>
+      <c r="CV189" t="str">
         <f t="shared" si="8"/>
-        <v>-8.6</v>
+        <v/>
       </c>
     </row>
     <row r="190" spans="1:100" x14ac:dyDescent="0.2">
@@ -20225,11 +20822,11 @@
       </c>
       <c r="CU191" t="str">
         <f t="shared" si="7"/>
-        <v>4_hydroxybenzaldehyde</v>
-      </c>
-      <c r="CV191">
+        <v/>
+      </c>
+      <c r="CV191" t="str">
         <f t="shared" si="8"/>
-        <v>-12.36</v>
+        <v/>
       </c>
     </row>
     <row r="192" spans="1:100" x14ac:dyDescent="0.2">
@@ -20580,11 +21177,11 @@
         <v>1</v>
       </c>
       <c r="CU195" t="str">
-        <f t="shared" ref="CU195:CU258" si="10">IF(ISNUMBER(CK195),A195,"")</f>
+        <f t="shared" ref="CU195:CU258" si="10">IF(ISNUMBER(CD195),A195,"")</f>
         <v/>
       </c>
       <c r="CV195" t="str">
-        <f t="shared" ref="CV195:CV258" si="11">IF(ISNUMBER(CK195),CK195,"")</f>
+        <f t="shared" ref="CV195:CV258" si="11">IF(ISNUMBER(CD195),CD195,"")</f>
         <v/>
       </c>
     </row>
@@ -21047,11 +21644,11 @@
       </c>
       <c r="CU200" t="str">
         <f t="shared" si="10"/>
-        <v>4_methylpyridine</v>
-      </c>
-      <c r="CV200">
+        <v/>
+      </c>
+      <c r="CV200" t="str">
         <f t="shared" si="11"/>
-        <v>-6.6</v>
+        <v/>
       </c>
     </row>
     <row r="201" spans="1:100" x14ac:dyDescent="0.2">
@@ -21270,11 +21867,11 @@
       </c>
       <c r="CU202" t="str">
         <f t="shared" si="10"/>
-        <v>4_nitroaniline</v>
-      </c>
-      <c r="CV202">
+        <v/>
+      </c>
+      <c r="CV202" t="str">
         <f t="shared" si="11"/>
-        <v>-11.35</v>
+        <v/>
       </c>
     </row>
     <row r="203" spans="1:100" x14ac:dyDescent="0.2">
@@ -21814,11 +22411,11 @@
       </c>
       <c r="CU207" t="str">
         <f t="shared" si="10"/>
-        <v>acetic_acid</v>
-      </c>
-      <c r="CV207">
+        <v/>
+      </c>
+      <c r="CV207" t="str">
         <f t="shared" si="11"/>
-        <v>-6.35</v>
+        <v/>
       </c>
     </row>
     <row r="208" spans="1:100" x14ac:dyDescent="0.2">
@@ -21946,7 +22543,7 @@
       </c>
       <c r="CV208">
         <f t="shared" si="11"/>
-        <v>-3.15</v>
+        <v>-4.63</v>
       </c>
     </row>
     <row r="209" spans="1:100" x14ac:dyDescent="0.2">
@@ -22083,7 +22680,7 @@
       </c>
       <c r="CV209">
         <f t="shared" si="11"/>
-        <v>-6.74</v>
+        <v>-7.63</v>
       </c>
     </row>
     <row r="210" spans="1:100" x14ac:dyDescent="0.2">
@@ -22335,11 +22932,11 @@
       </c>
       <c r="CU211" t="str">
         <f t="shared" si="10"/>
-        <v>aniline</v>
-      </c>
-      <c r="CV211">
+        <v/>
+      </c>
+      <c r="CV211" t="str">
         <f t="shared" si="11"/>
-        <v>-6.71</v>
+        <v/>
       </c>
     </row>
     <row r="212" spans="1:100" x14ac:dyDescent="0.2">
@@ -22461,7 +23058,7 @@
       </c>
       <c r="CV212">
         <f t="shared" si="11"/>
-        <v>-5.47</v>
+        <v>-6.18</v>
       </c>
     </row>
     <row r="213" spans="1:100" x14ac:dyDescent="0.2">
@@ -22604,7 +23201,7 @@
       </c>
       <c r="CV213">
         <f t="shared" si="11"/>
-        <v>-10.47</v>
+        <v>-11.24</v>
       </c>
     </row>
     <row r="214" spans="1:100" x14ac:dyDescent="0.2">
@@ -22821,7 +23418,7 @@
       </c>
       <c r="CV215">
         <f t="shared" si="11"/>
-        <v>-6.13</v>
+        <v>-7.13</v>
       </c>
     </row>
     <row r="216" spans="1:100" x14ac:dyDescent="0.2">
@@ -22939,11 +23536,11 @@
       </c>
       <c r="CU216" t="str">
         <f t="shared" si="10"/>
-        <v>benzamide</v>
-      </c>
-      <c r="CV216">
+        <v/>
+      </c>
+      <c r="CV216" t="str">
         <f t="shared" si="11"/>
-        <v>-11.77</v>
+        <v/>
       </c>
     </row>
     <row r="217" spans="1:100" x14ac:dyDescent="0.2">
@@ -23110,7 +23707,7 @@
       </c>
       <c r="CV217">
         <f t="shared" si="11"/>
-        <v>-3.72</v>
+        <v>-4.43</v>
       </c>
     </row>
     <row r="218" spans="1:100" x14ac:dyDescent="0.2">
@@ -23216,11 +23813,11 @@
       </c>
       <c r="CU218" t="str">
         <f t="shared" si="10"/>
-        <v>benzonitrile</v>
-      </c>
-      <c r="CV218">
+        <v/>
+      </c>
+      <c r="CV218" t="str">
         <f t="shared" si="11"/>
-        <v>-6.09</v>
+        <v/>
       </c>
     </row>
     <row r="219" spans="1:100" x14ac:dyDescent="0.2">
@@ -23428,7 +24025,7 @@
       </c>
       <c r="CV220">
         <f t="shared" si="11"/>
-        <v>-8.1199999999999992</v>
+        <v>-8.51</v>
       </c>
     </row>
     <row r="221" spans="1:100" x14ac:dyDescent="0.2">
@@ -23725,7 +24322,7 @@
       </c>
       <c r="CV223">
         <f t="shared" si="11"/>
-        <v>-8.18</v>
+        <v>-8.93</v>
       </c>
     </row>
     <row r="224" spans="1:100" x14ac:dyDescent="0.2">
@@ -23948,7 +24545,7 @@
       </c>
       <c r="CV225">
         <f t="shared" si="11"/>
-        <v>-62.61</v>
+        <v>-57.838999999999999</v>
       </c>
     </row>
     <row r="226" spans="1:100" x14ac:dyDescent="0.2">
@@ -24069,11 +24666,11 @@
       </c>
       <c r="CU226" t="str">
         <f t="shared" si="10"/>
-        <v>bromobenzene</v>
-      </c>
-      <c r="CV226">
+        <v/>
+      </c>
+      <c r="CV226" t="str">
         <f t="shared" si="11"/>
-        <v>-5.46</v>
+        <v/>
       </c>
     </row>
     <row r="227" spans="1:100" x14ac:dyDescent="0.2">
@@ -24177,7 +24774,7 @@
       </c>
       <c r="CV227">
         <f t="shared" si="11"/>
-        <v>-2.9</v>
+        <v>-3.38</v>
       </c>
     </row>
     <row r="228" spans="1:100" x14ac:dyDescent="0.2">
@@ -24277,11 +24874,11 @@
       </c>
       <c r="CU228" t="str">
         <f t="shared" si="10"/>
-        <v>bromoethane</v>
-      </c>
-      <c r="CV228">
+        <v/>
+      </c>
+      <c r="CV228" t="str">
         <f t="shared" si="11"/>
-        <v>-2.9</v>
+        <v/>
       </c>
     </row>
     <row r="229" spans="1:100" x14ac:dyDescent="0.2">
@@ -24369,11 +24966,11 @@
       </c>
       <c r="CU229" t="str">
         <f t="shared" si="10"/>
-        <v>bromomethane</v>
-      </c>
-      <c r="CV229">
+        <v/>
+      </c>
+      <c r="CV229" t="str">
         <f t="shared" si="11"/>
-        <v>-2.4300000000000002</v>
+        <v/>
       </c>
     </row>
     <row r="230" spans="1:100" x14ac:dyDescent="0.2">
@@ -24461,11 +25058,11 @@
       </c>
       <c r="CU230" t="str">
         <f t="shared" si="10"/>
-        <v>bromotrifluoromethane</v>
-      </c>
-      <c r="CV230">
+        <v/>
+      </c>
+      <c r="CV230" t="str">
         <f t="shared" si="11"/>
-        <v>-0.75</v>
+        <v/>
       </c>
     </row>
     <row r="231" spans="1:100" x14ac:dyDescent="0.2">
@@ -24562,11 +25159,11 @@
       </c>
       <c r="CU231" t="str">
         <f t="shared" si="10"/>
-        <v>but_1_ene</v>
-      </c>
-      <c r="CV231">
+        <v/>
+      </c>
+      <c r="CV231" t="str">
         <f t="shared" si="11"/>
-        <v>-1.89</v>
+        <v/>
       </c>
     </row>
     <row r="232" spans="1:100" x14ac:dyDescent="0.2">
@@ -24654,11 +25251,11 @@
       </c>
       <c r="CU232" t="str">
         <f t="shared" si="10"/>
-        <v>but_1_yne</v>
-      </c>
-      <c r="CV232">
+        <v/>
+      </c>
+      <c r="CV232" t="str">
         <f t="shared" si="11"/>
-        <v>-2.15</v>
+        <v/>
       </c>
     </row>
     <row r="233" spans="1:100" x14ac:dyDescent="0.2">
@@ -24922,11 +25519,11 @@
       </c>
       <c r="CU234" t="str">
         <f t="shared" si="10"/>
-        <v>butan_1_ol</v>
-      </c>
-      <c r="CV234">
+        <v/>
+      </c>
+      <c r="CV234" t="str">
         <f t="shared" si="11"/>
-        <v>-5.71</v>
+        <v/>
       </c>
     </row>
     <row r="235" spans="1:100" x14ac:dyDescent="0.2">
@@ -25106,11 +25703,11 @@
       </c>
       <c r="CU236" t="str">
         <f t="shared" si="10"/>
-        <v>butanenitrile</v>
-      </c>
-      <c r="CV236">
+        <v/>
+      </c>
+      <c r="CV236" t="str">
         <f t="shared" si="11"/>
-        <v>-4.25</v>
+        <v/>
       </c>
     </row>
     <row r="237" spans="1:100" x14ac:dyDescent="0.2">
@@ -25261,11 +25858,11 @@
       </c>
       <c r="CU237" t="str">
         <f t="shared" si="10"/>
-        <v>butanoic_acid</v>
-      </c>
-      <c r="CV237">
+        <v/>
+      </c>
+      <c r="CV237" t="str">
         <f t="shared" si="11"/>
-        <v>-7.58</v>
+        <v/>
       </c>
     </row>
     <row r="238" spans="1:100" x14ac:dyDescent="0.2">
@@ -25507,7 +26104,7 @@
       </c>
       <c r="CV238">
         <f t="shared" si="11"/>
-        <v>-3.78</v>
+        <v>-4.5599999999999996</v>
       </c>
     </row>
     <row r="239" spans="1:100" x14ac:dyDescent="0.2">
@@ -25595,11 +26192,11 @@
       </c>
       <c r="CU239" t="str">
         <f t="shared" si="10"/>
-        <v>butyraldehyde</v>
-      </c>
-      <c r="CV239">
+        <v/>
+      </c>
+      <c r="CV239" t="str">
         <f t="shared" si="11"/>
-        <v>-4.62</v>
+        <v/>
       </c>
     </row>
     <row r="240" spans="1:100" x14ac:dyDescent="0.2">
@@ -25739,7 +26336,7 @@
       </c>
       <c r="CV240">
         <f t="shared" si="11"/>
-        <v>-5</v>
+        <v>-5.54</v>
       </c>
     </row>
     <row r="241" spans="1:100" x14ac:dyDescent="0.2">
@@ -25926,7 +26523,7 @@
       </c>
       <c r="CV242">
         <f t="shared" si="11"/>
-        <v>-2.58</v>
+        <v>-2.74</v>
       </c>
     </row>
     <row r="243" spans="1:100" x14ac:dyDescent="0.2">
@@ -26014,11 +26611,11 @@
       </c>
       <c r="CU243" t="str">
         <f t="shared" si="10"/>
-        <v>chloroethylene</v>
-      </c>
-      <c r="CV243">
+        <v/>
+      </c>
+      <c r="CV243" t="str">
         <f t="shared" si="11"/>
-        <v>-2.66</v>
+        <v/>
       </c>
     </row>
     <row r="244" spans="1:100" x14ac:dyDescent="0.2">
@@ -26205,7 +26802,7 @@
       </c>
       <c r="CV245">
         <f t="shared" si="11"/>
-        <v>-1.79</v>
+        <v>-2.36</v>
       </c>
     </row>
     <row r="246" spans="1:100" x14ac:dyDescent="0.2">
@@ -26428,7 +27025,7 @@
       </c>
       <c r="CV247">
         <f t="shared" si="11"/>
-        <v>-68.19</v>
+        <v>-61.185000000000002</v>
       </c>
     </row>
     <row r="248" spans="1:100" x14ac:dyDescent="0.2">
@@ -26555,11 +27152,11 @@
       </c>
       <c r="CU248" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="CV248" t="str">
+        <v>Cs</v>
+      </c>
+      <c r="CV248">
         <f t="shared" si="11"/>
-        <v/>
+        <v>-75.765000000000001</v>
       </c>
     </row>
     <row r="249" spans="1:100" x14ac:dyDescent="0.2">
@@ -26972,7 +27569,7 @@
       </c>
       <c r="CV252">
         <f t="shared" si="11"/>
-        <v>-3.46</v>
+        <v>-3.15</v>
       </c>
     </row>
     <row r="253" spans="1:100" x14ac:dyDescent="0.2">
@@ -27419,11 +28016,11 @@
       </c>
       <c r="CU257" t="str">
         <f t="shared" si="10"/>
-        <v>cyclopentane</v>
-      </c>
-      <c r="CV257">
+        <v/>
+      </c>
+      <c r="CV257" t="str">
         <f t="shared" si="11"/>
-        <v>-2.65</v>
+        <v/>
       </c>
     </row>
     <row r="258" spans="1:100" x14ac:dyDescent="0.2">
@@ -27611,12 +28208,12 @@
         <v>4</v>
       </c>
       <c r="CU259" t="str">
-        <f t="shared" ref="CU259:CU322" si="13">IF(ISNUMBER(CK259),A259,"")</f>
-        <v>cyclopentanone</v>
-      </c>
-      <c r="CV259">
-        <f t="shared" ref="CV259:CV322" si="14">IF(ISNUMBER(CK259),CK259,"")</f>
-        <v>-5.01</v>
+        <f t="shared" ref="CU259:CU322" si="13">IF(ISNUMBER(CD259),A259,"")</f>
+        <v/>
+      </c>
+      <c r="CV259" t="str">
+        <f t="shared" ref="CV259:CV322" si="14">IF(ISNUMBER(CD259),CD259,"")</f>
+        <v/>
       </c>
     </row>
     <row r="260" spans="1:100" x14ac:dyDescent="0.2">
@@ -27796,11 +28393,11 @@
       </c>
       <c r="CU261" t="str">
         <f t="shared" si="13"/>
-        <v>cyclopropane</v>
-      </c>
-      <c r="CV261">
+        <v/>
+      </c>
+      <c r="CV261" t="str">
         <f t="shared" si="14"/>
-        <v>-1.6</v>
+        <v/>
       </c>
     </row>
     <row r="262" spans="1:100" x14ac:dyDescent="0.2">
@@ -27894,11 +28491,11 @@
       </c>
       <c r="CU262" t="str">
         <f t="shared" si="13"/>
-        <v>decan_1_ol</v>
-      </c>
-      <c r="CV262">
+        <v/>
+      </c>
+      <c r="CV262" t="str">
         <f t="shared" si="14"/>
-        <v>-9.8800000000000008</v>
+        <v/>
       </c>
     </row>
     <row r="263" spans="1:100" x14ac:dyDescent="0.2">
@@ -28612,11 +29209,11 @@
       </c>
       <c r="CU270" t="str">
         <f t="shared" si="13"/>
-        <v>dibromomethane</v>
-      </c>
-      <c r="CV270">
+        <v/>
+      </c>
+      <c r="CV270" t="str">
         <f t="shared" si="14"/>
-        <v>-4.18</v>
+        <v/>
       </c>
     </row>
     <row r="271" spans="1:100" x14ac:dyDescent="0.2">
@@ -28740,11 +29337,11 @@
       </c>
       <c r="CU271" t="str">
         <f t="shared" si="13"/>
-        <v>dichloromethane</v>
-      </c>
-      <c r="CV271">
+        <v/>
+      </c>
+      <c r="CV271" t="str">
         <f t="shared" si="14"/>
-        <v>-3.07</v>
+        <v/>
       </c>
     </row>
     <row r="272" spans="1:100" x14ac:dyDescent="0.2">
@@ -28927,11 +29524,11 @@
       </c>
       <c r="CU273" t="str">
         <f t="shared" si="13"/>
-        <v>diethyl_disulfide</v>
-      </c>
-      <c r="CV273">
+        <v/>
+      </c>
+      <c r="CV273" t="str">
         <f t="shared" si="14"/>
-        <v>-5.45</v>
+        <v/>
       </c>
     </row>
     <row r="274" spans="1:100" x14ac:dyDescent="0.2">
@@ -29043,11 +29640,11 @@
       </c>
       <c r="CU274" t="str">
         <f t="shared" si="13"/>
-        <v>diethyl_ether</v>
-      </c>
-      <c r="CV274">
+        <v/>
+      </c>
+      <c r="CV274" t="str">
         <f t="shared" si="14"/>
-        <v>-2.89</v>
+        <v/>
       </c>
     </row>
     <row r="275" spans="1:100" x14ac:dyDescent="0.2">
@@ -29319,11 +29916,11 @@
       </c>
       <c r="CU277" t="str">
         <f t="shared" si="13"/>
-        <v>diethyl_sulfide</v>
-      </c>
-      <c r="CV277">
+        <v/>
+      </c>
+      <c r="CV277" t="str">
         <f t="shared" si="14"/>
-        <v>-4.09</v>
+        <v/>
       </c>
     </row>
     <row r="278" spans="1:100" x14ac:dyDescent="0.2">
@@ -29453,11 +30050,11 @@
       </c>
       <c r="CU278" t="str">
         <f t="shared" si="13"/>
-        <v>diethylamine</v>
-      </c>
-      <c r="CV278">
+        <v/>
+      </c>
+      <c r="CV278" t="str">
         <f t="shared" si="14"/>
-        <v>-4.75</v>
+        <v/>
       </c>
     </row>
     <row r="279" spans="1:100" x14ac:dyDescent="0.2">
@@ -29548,11 +30145,11 @@
       </c>
       <c r="CU279" t="str">
         <f t="shared" si="13"/>
-        <v>diiodomethane</v>
-      </c>
-      <c r="CV279">
+        <v/>
+      </c>
+      <c r="CV279" t="str">
         <f t="shared" si="14"/>
-        <v>-5.63</v>
+        <v/>
       </c>
     </row>
     <row r="280" spans="1:100" x14ac:dyDescent="0.2">
@@ -29910,11 +30507,11 @@
       </c>
       <c r="CU283" t="str">
         <f t="shared" si="13"/>
-        <v>dimethyl_disulfide</v>
-      </c>
-      <c r="CV283">
+        <v/>
+      </c>
+      <c r="CV283" t="str">
         <f t="shared" si="14"/>
-        <v>-4.24</v>
+        <v/>
       </c>
     </row>
     <row r="284" spans="1:100" x14ac:dyDescent="0.2">
@@ -30005,11 +30602,11 @@
       </c>
       <c r="CU284" t="str">
         <f t="shared" si="13"/>
-        <v>dimethyl_ether</v>
-      </c>
-      <c r="CV284">
+        <v/>
+      </c>
+      <c r="CV284" t="str">
         <f t="shared" si="14"/>
-        <v>-2.06</v>
+        <v/>
       </c>
     </row>
     <row r="285" spans="1:100" x14ac:dyDescent="0.2">
@@ -30499,7 +31096,7 @@
       </c>
       <c r="CV289">
         <f t="shared" si="14"/>
-        <v>-2.72</v>
+        <v>-2.87</v>
       </c>
     </row>
     <row r="290" spans="1:100" x14ac:dyDescent="0.2">
@@ -31158,7 +31755,7 @@
       </c>
       <c r="CV296">
         <f t="shared" si="14"/>
-        <v>-0.64</v>
+        <v>-0.3</v>
       </c>
     </row>
     <row r="297" spans="1:100" x14ac:dyDescent="0.2">
@@ -31501,7 +32098,7 @@
       </c>
       <c r="CV298">
         <f t="shared" si="14"/>
-        <v>-4.3600000000000003</v>
+        <v>-5.23</v>
       </c>
     </row>
     <row r="299" spans="1:100" x14ac:dyDescent="0.2">
@@ -31592,11 +32189,11 @@
       </c>
       <c r="CU299" t="str">
         <f t="shared" si="13"/>
-        <v>ethene</v>
-      </c>
-      <c r="CV299">
+        <v/>
+      </c>
+      <c r="CV299" t="str">
         <f t="shared" si="14"/>
-        <v>-0.27</v>
+        <v/>
       </c>
     </row>
     <row r="300" spans="1:100" x14ac:dyDescent="0.2">
@@ -31769,7 +32366,7 @@
       </c>
       <c r="CV300">
         <f t="shared" si="14"/>
-        <v>-4.0599999999999996</v>
+        <v>-4.26</v>
       </c>
     </row>
     <row r="301" spans="1:100" x14ac:dyDescent="0.2">
@@ -31863,11 +32460,11 @@
       </c>
       <c r="CU301" t="str">
         <f t="shared" si="13"/>
-        <v>ethyl_benzoate</v>
-      </c>
-      <c r="CV301">
+        <v/>
+      </c>
+      <c r="CV301" t="str">
         <f t="shared" si="14"/>
-        <v>-7.24</v>
+        <v/>
       </c>
     </row>
     <row r="302" spans="1:100" x14ac:dyDescent="0.2">
@@ -32323,11 +32920,11 @@
       </c>
       <c r="CU306" t="str">
         <f t="shared" si="13"/>
-        <v>ethyl_phenyl_ether</v>
-      </c>
-      <c r="CV306">
+        <v/>
+      </c>
+      <c r="CV306" t="str">
         <f t="shared" si="14"/>
-        <v>-5.65</v>
+        <v/>
       </c>
     </row>
     <row r="307" spans="1:100" x14ac:dyDescent="0.2">
@@ -32564,11 +33161,11 @@
       </c>
       <c r="CU308" t="str">
         <f t="shared" si="13"/>
-        <v>ethylamine</v>
-      </c>
-      <c r="CV308">
+        <v/>
+      </c>
+      <c r="CV308" t="str">
         <f t="shared" si="14"/>
-        <v>-4.09</v>
+        <v/>
       </c>
     </row>
     <row r="309" spans="1:100" x14ac:dyDescent="0.2">
@@ -32683,11 +33280,11 @@
       </c>
       <c r="CU309" t="str">
         <f t="shared" si="13"/>
-        <v>ethylbenzene</v>
-      </c>
-      <c r="CV309">
+        <v/>
+      </c>
+      <c r="CV309" t="str">
         <f t="shared" si="14"/>
-        <v>-5.08</v>
+        <v/>
       </c>
     </row>
     <row r="310" spans="1:100" x14ac:dyDescent="0.2">
@@ -32894,11 +33491,11 @@
       </c>
       <c r="CU311" t="str">
         <f t="shared" si="13"/>
-        <v>fluorobenzene</v>
-      </c>
-      <c r="CV311">
+        <v/>
+      </c>
+      <c r="CV311" t="str">
         <f t="shared" si="14"/>
-        <v>-3.87</v>
+        <v/>
       </c>
     </row>
     <row r="312" spans="1:100" x14ac:dyDescent="0.2">
@@ -33093,11 +33690,11 @@
       </c>
       <c r="CU313" t="str">
         <f t="shared" si="13"/>
-        <v>formaldehyde</v>
-      </c>
-      <c r="CV313">
+        <v/>
+      </c>
+      <c r="CV313" t="str">
         <f t="shared" si="14"/>
-        <v>-3.23</v>
+        <v/>
       </c>
     </row>
     <row r="314" spans="1:100" x14ac:dyDescent="0.2">
@@ -33512,11 +34109,11 @@
       </c>
       <c r="CU317" t="str">
         <f t="shared" si="13"/>
-        <v>heptan_1_ol</v>
-      </c>
-      <c r="CV317">
+        <v/>
+      </c>
+      <c r="CV317" t="str">
         <f t="shared" si="14"/>
-        <v>-7.75</v>
+        <v/>
       </c>
     </row>
     <row r="318" spans="1:100" x14ac:dyDescent="0.2">
@@ -33649,11 +34246,11 @@
       </c>
       <c r="CU318" t="str">
         <f t="shared" si="13"/>
-        <v>heptan_2_one</v>
-      </c>
-      <c r="CV318">
+        <v/>
+      </c>
+      <c r="CV318" t="str">
         <f t="shared" si="14"/>
-        <v>-5.65</v>
+        <v/>
       </c>
     </row>
     <row r="319" spans="1:100" x14ac:dyDescent="0.2">
@@ -33925,11 +34522,11 @@
       </c>
       <c r="CU321" t="str">
         <f t="shared" si="13"/>
-        <v>hex_1_ene</v>
-      </c>
-      <c r="CV321">
+        <v/>
+      </c>
+      <c r="CV321" t="str">
         <f t="shared" si="14"/>
-        <v>-2.94</v>
+        <v/>
       </c>
     </row>
     <row r="322" spans="1:100" x14ac:dyDescent="0.2">
@@ -34020,11 +34617,11 @@
       </c>
       <c r="CU322" t="str">
         <f t="shared" si="13"/>
-        <v>hex_1_yne</v>
-      </c>
-      <c r="CV322">
+        <v/>
+      </c>
+      <c r="CV322" t="str">
         <f t="shared" si="14"/>
-        <v>-3.43</v>
+        <v/>
       </c>
     </row>
     <row r="323" spans="1:100" x14ac:dyDescent="0.2">
@@ -34108,11 +34705,11 @@
         <v>1</v>
       </c>
       <c r="CU323" t="str">
-        <f t="shared" ref="CU323:CU386" si="16">IF(ISNUMBER(CK323),A323,"")</f>
+        <f t="shared" ref="CU323:CU386" si="16">IF(ISNUMBER(CD323),A323,"")</f>
         <v/>
       </c>
       <c r="CV323" t="str">
-        <f t="shared" ref="CV323:CV386" si="17">IF(ISNUMBER(CK323),CK323,"")</f>
+        <f t="shared" ref="CV323:CV386" si="17">IF(ISNUMBER(CD323),CD323,"")</f>
         <v/>
       </c>
     </row>
@@ -34359,11 +34956,11 @@
       </c>
       <c r="CU325" t="str">
         <f t="shared" si="16"/>
-        <v>hexan_1_ol</v>
-      </c>
-      <c r="CV325">
+        <v/>
+      </c>
+      <c r="CV325" t="str">
         <f t="shared" si="17"/>
-        <v>-7.06</v>
+        <v/>
       </c>
     </row>
     <row r="326" spans="1:100" x14ac:dyDescent="0.2">
@@ -34502,11 +35099,11 @@
       </c>
       <c r="CU326" t="str">
         <f t="shared" si="16"/>
-        <v>hexan_2_one</v>
-      </c>
-      <c r="CV326">
+        <v/>
+      </c>
+      <c r="CV326" t="str">
         <f t="shared" si="17"/>
-        <v>-5.0199999999999996</v>
+        <v/>
       </c>
     </row>
     <row r="327" spans="1:100" x14ac:dyDescent="0.2">
@@ -34808,11 +35405,11 @@
       </c>
       <c r="CU329" t="str">
         <f t="shared" si="16"/>
-        <v>hexanoic_acid</v>
-      </c>
-      <c r="CV329">
+        <v/>
+      </c>
+      <c r="CV329" t="str">
         <f t="shared" si="17"/>
-        <v>-8.82</v>
+        <v/>
       </c>
     </row>
     <row r="330" spans="1:100" x14ac:dyDescent="0.2">
@@ -34906,11 +35503,11 @@
       </c>
       <c r="CU330" t="str">
         <f t="shared" si="16"/>
-        <v>hydrazine</v>
-      </c>
-      <c r="CV330">
+        <v/>
+      </c>
+      <c r="CV330" t="str">
         <f t="shared" si="17"/>
-        <v>-3.44</v>
+        <v/>
       </c>
     </row>
     <row r="331" spans="1:100" x14ac:dyDescent="0.2">
@@ -35142,7 +35739,7 @@
       </c>
       <c r="CV332">
         <f t="shared" si="17"/>
-        <v>-54.77</v>
+        <v>-53.298000000000002</v>
       </c>
     </row>
     <row r="333" spans="1:100" x14ac:dyDescent="0.2">
@@ -35445,7 +36042,7 @@
       </c>
       <c r="CV335">
         <f t="shared" si="17"/>
-        <v>-6.18</v>
+        <v>-6.76</v>
       </c>
     </row>
     <row r="336" spans="1:100" x14ac:dyDescent="0.2">
@@ -35552,7 +36149,7 @@
       </c>
       <c r="CV336">
         <f t="shared" si="17"/>
-        <v>-3.45</v>
+        <v>-3.92</v>
       </c>
     </row>
     <row r="337" spans="1:100" x14ac:dyDescent="0.2">
@@ -35649,11 +36246,11 @@
       </c>
       <c r="CU337" t="str">
         <f t="shared" si="16"/>
-        <v>iodoethane</v>
-      </c>
-      <c r="CV337">
+        <v/>
+      </c>
+      <c r="CV337" t="str">
         <f t="shared" si="17"/>
-        <v>-3.45</v>
+        <v/>
       </c>
     </row>
     <row r="338" spans="1:100" x14ac:dyDescent="0.2">
@@ -35766,7 +36363,7 @@
       </c>
       <c r="CV338">
         <f t="shared" si="17"/>
-        <v>-3.07</v>
+        <v>-3.49</v>
       </c>
     </row>
     <row r="339" spans="1:100" x14ac:dyDescent="0.2">
@@ -36879,7 +37476,7 @@
       </c>
       <c r="CV350">
         <f t="shared" si="17"/>
-        <v>-80.930000000000007</v>
+        <v>-86.52</v>
       </c>
     </row>
     <row r="351" spans="1:100" x14ac:dyDescent="0.2">
@@ -37007,7 +37604,7 @@
       </c>
       <c r="CV351">
         <f t="shared" si="17"/>
-        <v>-123.89</v>
+        <v>-128.82400000000001</v>
       </c>
     </row>
     <row r="352" spans="1:100" x14ac:dyDescent="0.2">
@@ -37235,11 +37832,11 @@
       </c>
       <c r="CU353" t="str">
         <f t="shared" si="16"/>
-        <v>m_cresol</v>
-      </c>
-      <c r="CV353">
+        <v/>
+      </c>
+      <c r="CV353" t="str">
         <f t="shared" si="17"/>
-        <v>-8.1999999999999993</v>
+        <v/>
       </c>
     </row>
     <row r="354" spans="1:100" x14ac:dyDescent="0.2">
@@ -37370,7 +37967,7 @@
       </c>
       <c r="CV354">
         <f t="shared" si="17"/>
-        <v>-5.25</v>
+        <v>-5.17</v>
       </c>
     </row>
     <row r="355" spans="1:100" x14ac:dyDescent="0.2">
@@ -37461,11 +38058,11 @@
       </c>
       <c r="CU355" t="str">
         <f t="shared" si="16"/>
-        <v>methane</v>
-      </c>
-      <c r="CV355">
+        <v/>
+      </c>
+      <c r="CV355" t="str">
         <f t="shared" si="17"/>
-        <v>0.51</v>
+        <v/>
       </c>
     </row>
     <row r="356" spans="1:100" x14ac:dyDescent="0.2">
@@ -37825,7 +38422,7 @@
       </c>
       <c r="CV358">
         <f t="shared" si="17"/>
-        <v>-3.87</v>
+        <v>-4.6500000000000004</v>
       </c>
     </row>
     <row r="359" spans="1:100" x14ac:dyDescent="0.2">
@@ -38071,11 +38668,11 @@
       </c>
       <c r="CU360" t="str">
         <f t="shared" si="16"/>
-        <v>methyl_acetate</v>
-      </c>
-      <c r="CV360">
+        <v/>
+      </c>
+      <c r="CV360" t="str">
         <f t="shared" si="17"/>
-        <v>-3.54</v>
+        <v/>
       </c>
     </row>
     <row r="361" spans="1:100" x14ac:dyDescent="0.2">
@@ -38190,11 +38787,11 @@
       </c>
       <c r="CU361" t="str">
         <f t="shared" si="16"/>
-        <v>methyl_benzoate</v>
-      </c>
-      <c r="CV361">
+        <v/>
+      </c>
+      <c r="CV361" t="str">
         <f t="shared" si="17"/>
-        <v>-7.26</v>
+        <v/>
       </c>
     </row>
     <row r="362" spans="1:100" x14ac:dyDescent="0.2">
@@ -38285,11 +38882,11 @@
       </c>
       <c r="CU362" t="str">
         <f t="shared" si="16"/>
-        <v>methyl_butanoate</v>
-      </c>
-      <c r="CV362">
+        <v/>
+      </c>
+      <c r="CV362" t="str">
         <f t="shared" si="17"/>
-        <v>-4.59</v>
+        <v/>
       </c>
     </row>
     <row r="363" spans="1:100" x14ac:dyDescent="0.2">
@@ -39092,11 +39689,11 @@
       </c>
       <c r="CU371" t="str">
         <f t="shared" si="16"/>
-        <v>methyl_formate</v>
-      </c>
-      <c r="CV371">
+        <v/>
+      </c>
+      <c r="CV371" t="str">
         <f t="shared" si="17"/>
-        <v>-2.82</v>
+        <v/>
       </c>
     </row>
     <row r="372" spans="1:100" x14ac:dyDescent="0.2">
@@ -39312,11 +39909,11 @@
       </c>
       <c r="CU373" t="str">
         <f t="shared" si="16"/>
-        <v>methyl_isopropyl_ether</v>
-      </c>
-      <c r="CV373">
+        <v/>
+      </c>
+      <c r="CV373" t="str">
         <f t="shared" si="17"/>
-        <v>-4.6399999999999997</v>
+        <v/>
       </c>
     </row>
     <row r="374" spans="1:100" x14ac:dyDescent="0.2">
@@ -39811,11 +40408,11 @@
       </c>
       <c r="CU378" t="str">
         <f t="shared" si="16"/>
-        <v>methyl_pentanoate</v>
-      </c>
-      <c r="CV378">
+        <v/>
+      </c>
+      <c r="CV378" t="str">
         <f t="shared" si="17"/>
-        <v>-5.13</v>
+        <v/>
       </c>
     </row>
     <row r="379" spans="1:100" x14ac:dyDescent="0.2">
@@ -39954,11 +40551,11 @@
       </c>
       <c r="CU379" t="str">
         <f t="shared" si="16"/>
-        <v>methyl_propanoate</v>
-      </c>
-      <c r="CV379">
+        <v/>
+      </c>
+      <c r="CV379" t="str">
         <f t="shared" si="17"/>
-        <v>-4.0599999999999996</v>
+        <v/>
       </c>
     </row>
     <row r="380" spans="1:100" x14ac:dyDescent="0.2">
@@ -40046,11 +40643,11 @@
       </c>
       <c r="CU380" t="str">
         <f t="shared" si="16"/>
-        <v>methyl_propyl_ether</v>
-      </c>
-      <c r="CV380">
+        <v/>
+      </c>
+      <c r="CV380" t="str">
         <f t="shared" si="17"/>
-        <v>-3.63</v>
+        <v/>
       </c>
     </row>
     <row r="381" spans="1:100" x14ac:dyDescent="0.2">
@@ -40525,7 +41122,7 @@
       </c>
       <c r="CV385">
         <f t="shared" si="17"/>
-        <v>-3.78</v>
+        <v>-2.66</v>
       </c>
     </row>
     <row r="386" spans="1:100" x14ac:dyDescent="0.2">
@@ -40698,11 +41295,11 @@
         <v>1</v>
       </c>
       <c r="CU387" t="str">
-        <f t="shared" ref="CU387:CU450" si="19">IF(ISNUMBER(CK387),A387,"")</f>
+        <f t="shared" ref="CU387:CU450" si="19">IF(ISNUMBER(CD387),A387,"")</f>
         <v/>
       </c>
       <c r="CV387" t="str">
-        <f t="shared" ref="CV387:CV450" si="20">IF(ISNUMBER(CK387),CK387,"")</f>
+        <f t="shared" ref="CV387:CV450" si="20">IF(ISNUMBER(CD387),CD387,"")</f>
         <v/>
       </c>
     </row>
@@ -40791,11 +41388,11 @@
       </c>
       <c r="CU388" t="str">
         <f t="shared" si="19"/>
-        <v>morpholine</v>
-      </c>
-      <c r="CV388">
+        <v/>
+      </c>
+      <c r="CV388" t="str">
         <f t="shared" si="20"/>
-        <v>-5.99</v>
+        <v/>
       </c>
     </row>
     <row r="389" spans="1:100" x14ac:dyDescent="0.2">
@@ -41003,7 +41600,7 @@
       </c>
       <c r="CV390">
         <f t="shared" si="20"/>
-        <v>-1.86</v>
+        <v>-1.48</v>
       </c>
     </row>
     <row r="391" spans="1:100" x14ac:dyDescent="0.2">
@@ -41252,11 +41849,11 @@
       </c>
       <c r="CU392" t="str">
         <f t="shared" si="19"/>
-        <v>n_butyl_acetate</v>
-      </c>
-      <c r="CV392">
+        <v/>
+      </c>
+      <c r="CV392" t="str">
         <f t="shared" si="20"/>
-        <v>-4.96</v>
+        <v/>
       </c>
     </row>
     <row r="393" spans="1:100" x14ac:dyDescent="0.2">
@@ -41490,11 +42087,11 @@
       </c>
       <c r="CU394" t="str">
         <f t="shared" si="19"/>
-        <v>n_butylamine</v>
-      </c>
-      <c r="CV394">
+        <v/>
+      </c>
+      <c r="CV394" t="str">
         <f t="shared" si="20"/>
-        <v>-5.33</v>
+        <v/>
       </c>
     </row>
     <row r="395" spans="1:100" x14ac:dyDescent="0.2">
@@ -41821,7 +42418,7 @@
       </c>
       <c r="CV397">
         <f t="shared" si="20"/>
-        <v>-3.74</v>
+        <v>-3.16</v>
       </c>
     </row>
     <row r="398" spans="1:100" x14ac:dyDescent="0.2">
@@ -42059,7 +42656,7 @@
       </c>
       <c r="CV399">
         <f t="shared" si="20"/>
-        <v>-3.01</v>
+        <v>-2.72</v>
       </c>
     </row>
     <row r="400" spans="1:100" x14ac:dyDescent="0.2">
@@ -42503,11 +43100,11 @@
       </c>
       <c r="CU404" t="str">
         <f t="shared" si="19"/>
-        <v>N_methylacetamide</v>
-      </c>
-      <c r="CV404">
+        <v/>
+      </c>
+      <c r="CV404" t="str">
         <f t="shared" si="20"/>
-        <v>-8.57</v>
+        <v/>
       </c>
     </row>
     <row r="405" spans="1:100" x14ac:dyDescent="0.2">
@@ -42610,11 +43207,11 @@
       </c>
       <c r="CU405" t="str">
         <f t="shared" si="19"/>
-        <v>N_methylaniline</v>
-      </c>
-      <c r="CV405">
+        <v/>
+      </c>
+      <c r="CV405" t="str">
         <f t="shared" si="20"/>
-        <v>-6.94</v>
+        <v/>
       </c>
     </row>
     <row r="406" spans="1:100" x14ac:dyDescent="0.2">
@@ -42969,11 +43566,11 @@
       </c>
       <c r="CU409" t="str">
         <f t="shared" si="19"/>
-        <v>n_nonane</v>
-      </c>
-      <c r="CV409">
+        <v/>
+      </c>
+      <c r="CV409" t="str">
         <f t="shared" si="20"/>
-        <v>-4.55</v>
+        <v/>
       </c>
     </row>
     <row r="410" spans="1:100" x14ac:dyDescent="0.2">
@@ -43206,7 +43803,7 @@
       </c>
       <c r="CV410">
         <f t="shared" si="20"/>
-        <v>-4.18</v>
+        <v>-3.77</v>
       </c>
     </row>
     <row r="411" spans="1:100" x14ac:dyDescent="0.2">
@@ -43441,7 +44038,7 @@
       </c>
       <c r="CV412">
         <f t="shared" si="20"/>
-        <v>-2.4500000000000002</v>
+        <v>-2.0699999999999998</v>
       </c>
     </row>
     <row r="413" spans="1:100" x14ac:dyDescent="0.2">
@@ -43983,11 +44580,11 @@
       </c>
       <c r="CU418" t="str">
         <f t="shared" si="19"/>
-        <v>n_propanethiol</v>
-      </c>
-      <c r="CV418">
+        <v/>
+      </c>
+      <c r="CV418" t="str">
         <f t="shared" si="20"/>
-        <v>-3.52</v>
+        <v/>
       </c>
     </row>
     <row r="419" spans="1:100" x14ac:dyDescent="0.2">
@@ -44132,11 +44729,11 @@
       </c>
       <c r="CU419" t="str">
         <f t="shared" si="19"/>
-        <v>n_propyl_acetate</v>
-      </c>
-      <c r="CV419">
+        <v/>
+      </c>
+      <c r="CV419" t="str">
         <f t="shared" si="20"/>
-        <v>-4.55</v>
+        <v/>
       </c>
     </row>
     <row r="420" spans="1:100" x14ac:dyDescent="0.2">
@@ -44545,11 +45142,11 @@
       </c>
       <c r="CU423" t="str">
         <f t="shared" si="19"/>
-        <v>n_propylamine</v>
-      </c>
-      <c r="CV423">
+        <v/>
+      </c>
+      <c r="CV423" t="str">
         <f t="shared" si="20"/>
-        <v>-4.7699999999999996</v>
+        <v/>
       </c>
     </row>
     <row r="424" spans="1:100" x14ac:dyDescent="0.2">
@@ -44861,7 +45458,7 @@
       </c>
       <c r="CV426">
         <f t="shared" si="20"/>
-        <v>-98.26</v>
+        <v>-103.72799999999999</v>
       </c>
     </row>
     <row r="427" spans="1:100" x14ac:dyDescent="0.2">
@@ -45007,7 +45604,7 @@
       </c>
       <c r="CV427">
         <f t="shared" si="20"/>
-        <v>-6.97</v>
+        <v>-7.78</v>
       </c>
     </row>
     <row r="428" spans="1:100" x14ac:dyDescent="0.2">
@@ -45134,11 +45731,11 @@
       </c>
       <c r="CU428" t="str">
         <f t="shared" si="19"/>
-        <v>nitrobenzene</v>
-      </c>
-      <c r="CV428">
+        <v/>
+      </c>
+      <c r="CV428" t="str">
         <f t="shared" si="20"/>
-        <v>-6.63</v>
+        <v/>
       </c>
     </row>
     <row r="429" spans="1:100" x14ac:dyDescent="0.2">
@@ -45235,11 +45832,11 @@
       </c>
       <c r="CU429" t="str">
         <f t="shared" si="19"/>
-        <v>nitroethane</v>
-      </c>
-      <c r="CV429">
+        <v/>
+      </c>
+      <c r="CV429" t="str">
         <f t="shared" si="20"/>
-        <v>-3.93</v>
+        <v/>
       </c>
     </row>
     <row r="430" spans="1:100" x14ac:dyDescent="0.2">
@@ -45460,7 +46057,7 @@
       </c>
       <c r="CV430">
         <f t="shared" si="20"/>
-        <v>-3.51</v>
+        <v>-5.66</v>
       </c>
     </row>
     <row r="431" spans="1:100" x14ac:dyDescent="0.2">
@@ -45910,11 +46507,11 @@
       </c>
       <c r="CU435" t="str">
         <f t="shared" si="19"/>
-        <v>NN_dimethylformamide</v>
-      </c>
-      <c r="CV435">
+        <v/>
+      </c>
+      <c r="CV435" t="str">
         <f t="shared" si="20"/>
-        <v>-6.14</v>
+        <v/>
       </c>
     </row>
     <row r="436" spans="1:100" x14ac:dyDescent="0.2">
@@ -46513,11 +47110,11 @@
       </c>
       <c r="CU441" t="str">
         <f t="shared" si="19"/>
-        <v>o_cresol</v>
-      </c>
-      <c r="CV441">
+        <v/>
+      </c>
+      <c r="CV441" t="str">
         <f t="shared" si="20"/>
-        <v>-8.49</v>
+        <v/>
       </c>
     </row>
     <row r="442" spans="1:100" x14ac:dyDescent="0.2">
@@ -46712,11 +47309,11 @@
       </c>
       <c r="CU443" t="str">
         <f t="shared" si="19"/>
-        <v>o_xylene</v>
-      </c>
-      <c r="CV443">
+        <v/>
+      </c>
+      <c r="CV443" t="str">
         <f t="shared" si="20"/>
-        <v>-5.07</v>
+        <v/>
       </c>
     </row>
     <row r="444" spans="1:100" x14ac:dyDescent="0.2">
@@ -47000,11 +47597,11 @@
       </c>
       <c r="CU446" t="str">
         <f t="shared" si="19"/>
-        <v>octan_1_ol</v>
-      </c>
-      <c r="CV446">
+        <v/>
+      </c>
+      <c r="CV446" t="str">
         <f t="shared" si="20"/>
-        <v>-8.1300000000000008</v>
+        <v/>
       </c>
     </row>
     <row r="447" spans="1:100" x14ac:dyDescent="0.2">
@@ -47098,11 +47695,11 @@
       </c>
       <c r="CU447" t="str">
         <f t="shared" si="19"/>
-        <v>octan_2_one</v>
-      </c>
-      <c r="CV447">
+        <v/>
+      </c>
+      <c r="CV447" t="str">
         <f t="shared" si="20"/>
-        <v>-6.38</v>
+        <v/>
       </c>
     </row>
     <row r="448" spans="1:100" x14ac:dyDescent="0.2">
@@ -47361,7 +47958,7 @@
       </c>
       <c r="CV449">
         <f t="shared" si="20"/>
-        <v>-8.84</v>
+        <v>-8.35</v>
       </c>
     </row>
     <row r="450" spans="1:100" x14ac:dyDescent="0.2">
@@ -47543,12 +48140,12 @@
         <v>4</v>
       </c>
       <c r="CU451" t="str">
-        <f t="shared" ref="CU451:CU513" si="22">IF(ISNUMBER(CK451),A451,"")</f>
-        <v>p_toluidine</v>
-      </c>
-      <c r="CV451">
-        <f t="shared" ref="CV451:CV513" si="23">IF(ISNUMBER(CK451),CK451,"")</f>
-        <v>-7.46</v>
+        <f t="shared" ref="CU451:CU513" si="22">IF(ISNUMBER(CD451),A451,"")</f>
+        <v/>
+      </c>
+      <c r="CV451" t="str">
+        <f t="shared" ref="CV451:CV513" si="23">IF(ISNUMBER(CD451),CD451,"")</f>
+        <v/>
       </c>
     </row>
     <row r="452" spans="1:100" x14ac:dyDescent="0.2">
@@ -47670,7 +48267,7 @@
       </c>
       <c r="CV452">
         <f t="shared" si="23"/>
-        <v>-5.19</v>
+        <v>-5.5</v>
       </c>
     </row>
     <row r="453" spans="1:100" x14ac:dyDescent="0.2">
@@ -47856,11 +48453,11 @@
       </c>
       <c r="CU454" t="str">
         <f t="shared" si="22"/>
-        <v>pent_1_yne</v>
-      </c>
-      <c r="CV454">
+        <v/>
+      </c>
+      <c r="CV454" t="str">
         <f t="shared" si="23"/>
-        <v>-2.79</v>
+        <v/>
       </c>
     </row>
     <row r="455" spans="1:100" x14ac:dyDescent="0.2">
@@ -48037,11 +48634,11 @@
       </c>
       <c r="CU456" t="str">
         <f t="shared" si="22"/>
-        <v>pentachloroethane</v>
-      </c>
-      <c r="CV456">
+        <v/>
+      </c>
+      <c r="CV456" t="str">
         <f t="shared" si="23"/>
-        <v>-5.78</v>
+        <v/>
       </c>
     </row>
     <row r="457" spans="1:100" x14ac:dyDescent="0.2">
@@ -48198,11 +48795,11 @@
       </c>
       <c r="CU457" t="str">
         <f t="shared" si="22"/>
-        <v>pentan_1_ol</v>
-      </c>
-      <c r="CV457">
+        <v/>
+      </c>
+      <c r="CV457" t="str">
         <f t="shared" si="23"/>
-        <v>-6.4</v>
+        <v/>
       </c>
     </row>
     <row r="458" spans="1:100" x14ac:dyDescent="0.2">
@@ -48427,11 +49024,11 @@
       </c>
       <c r="CU459" t="str">
         <f t="shared" si="22"/>
-        <v>pentan_2_one</v>
-      </c>
-      <c r="CV459">
+        <v/>
+      </c>
+      <c r="CV459" t="str">
         <f t="shared" si="23"/>
-        <v>-4.3499999999999996</v>
+        <v/>
       </c>
     </row>
     <row r="460" spans="1:100" x14ac:dyDescent="0.2">
@@ -48614,11 +49211,11 @@
       </c>
       <c r="CU461" t="str">
         <f t="shared" si="22"/>
-        <v>pentan_3_one</v>
-      </c>
-      <c r="CV461">
+        <v/>
+      </c>
+      <c r="CV461" t="str">
         <f t="shared" si="23"/>
-        <v>-4.3600000000000003</v>
+        <v/>
       </c>
     </row>
     <row r="462" spans="1:100" x14ac:dyDescent="0.2">
@@ -48932,11 +49529,11 @@
       </c>
       <c r="CU464" t="str">
         <f t="shared" si="22"/>
-        <v>pentanoic_acid</v>
-      </c>
-      <c r="CV464">
+        <v/>
+      </c>
+      <c r="CV464" t="str">
         <f t="shared" si="23"/>
-        <v>-8.2200000000000006</v>
+        <v/>
       </c>
     </row>
     <row r="465" spans="1:100" x14ac:dyDescent="0.2">
@@ -49070,7 +49667,7 @@
       </c>
       <c r="CV465">
         <f t="shared" si="23"/>
-        <v>-10.039999999999999</v>
+        <v>-11.52</v>
       </c>
     </row>
     <row r="466" spans="1:100" x14ac:dyDescent="0.2">
@@ -49269,11 +49866,11 @@
       </c>
       <c r="CU466" t="str">
         <f t="shared" si="22"/>
-        <v>phenol</v>
-      </c>
-      <c r="CV466">
+        <v/>
+      </c>
+      <c r="CV466" t="str">
         <f t="shared" si="23"/>
-        <v>-8.69</v>
+        <v/>
       </c>
     </row>
     <row r="467" spans="1:100" x14ac:dyDescent="0.2">
@@ -49631,11 +50228,11 @@
       </c>
       <c r="CU470" t="str">
         <f t="shared" si="22"/>
-        <v>piperazine</v>
-      </c>
-      <c r="CV470">
+        <v/>
+      </c>
+      <c r="CV470" t="str">
         <f t="shared" si="23"/>
-        <v>-5.8</v>
+        <v/>
       </c>
     </row>
     <row r="471" spans="1:100" x14ac:dyDescent="0.2">
@@ -49735,11 +50332,11 @@
       </c>
       <c r="CU471" t="str">
         <f t="shared" si="22"/>
-        <v>piperidine</v>
-      </c>
-      <c r="CV471">
+        <v/>
+      </c>
+      <c r="CV471" t="str">
         <f t="shared" si="23"/>
-        <v>-6.27</v>
+        <v/>
       </c>
     </row>
     <row r="472" spans="1:100" x14ac:dyDescent="0.2">
@@ -50013,7 +50610,7 @@
       </c>
       <c r="CV473">
         <f t="shared" si="23"/>
-        <v>-5.0199999999999996</v>
+        <v>-5.56</v>
       </c>
     </row>
     <row r="474" spans="1:100" x14ac:dyDescent="0.2">
@@ -50212,7 +50809,7 @@
       </c>
       <c r="CV475">
         <f t="shared" si="23"/>
-        <v>-1.26</v>
+        <v>-0.87</v>
       </c>
     </row>
     <row r="476" spans="1:100" x14ac:dyDescent="0.2">
@@ -50628,11 +51225,11 @@
       </c>
       <c r="CU478" t="str">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="CV478" t="str">
+        <v>propanone</v>
+      </c>
+      <c r="CV478">
         <f t="shared" si="23"/>
-        <v/>
+        <v>-4.0199999999999996</v>
       </c>
     </row>
     <row r="479" spans="1:100" x14ac:dyDescent="0.2">
@@ -51051,7 +51648,7 @@
       </c>
       <c r="CV482">
         <f t="shared" si="23"/>
-        <v>-11.16</v>
+        <v>-13.17</v>
       </c>
     </row>
     <row r="483" spans="1:100" x14ac:dyDescent="0.2">
@@ -51199,11 +51796,11 @@
       </c>
       <c r="CU483" t="str">
         <f t="shared" si="22"/>
-        <v>pyridine</v>
-      </c>
-      <c r="CV483">
+        <v/>
+      </c>
+      <c r="CV483" t="str">
         <f t="shared" si="23"/>
-        <v>-5.34</v>
+        <v/>
       </c>
     </row>
     <row r="484" spans="1:100" x14ac:dyDescent="0.2">
@@ -51294,11 +51891,11 @@
       </c>
       <c r="CU484" t="str">
         <f t="shared" si="22"/>
-        <v>pyrrole</v>
-      </c>
-      <c r="CV484">
+        <v/>
+      </c>
+      <c r="CV484" t="str">
         <f t="shared" si="23"/>
-        <v>-5.28</v>
+        <v/>
       </c>
     </row>
     <row r="485" spans="1:100" x14ac:dyDescent="0.2">
@@ -51478,11 +52075,11 @@
       </c>
       <c r="CU486" t="str">
         <f t="shared" si="22"/>
-        <v>quinoline</v>
-      </c>
-      <c r="CV486">
+        <v/>
+      </c>
+      <c r="CV486" t="str">
         <f t="shared" si="23"/>
-        <v>-8.43</v>
+        <v/>
       </c>
     </row>
     <row r="487" spans="1:100" x14ac:dyDescent="0.2">
@@ -51609,11 +52206,11 @@
       </c>
       <c r="CU487" t="str">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="CV487" t="str">
+        <v>Rb</v>
+      </c>
+      <c r="CV487">
         <f t="shared" si="23"/>
-        <v/>
+        <v>-81.022999999999996</v>
       </c>
     </row>
     <row r="488" spans="1:100" x14ac:dyDescent="0.2">
@@ -52060,11 +52657,11 @@
       </c>
       <c r="CU492" t="str">
         <f t="shared" si="22"/>
-        <v>tetrachloroethene</v>
-      </c>
-      <c r="CV492">
+        <v/>
+      </c>
+      <c r="CV492" t="str">
         <f t="shared" si="23"/>
-        <v>-4.24</v>
+        <v/>
       </c>
     </row>
     <row r="493" spans="1:100" x14ac:dyDescent="0.2">
@@ -52170,11 +52767,11 @@
       </c>
       <c r="CU493" t="str">
         <f t="shared" si="22"/>
-        <v>tetrachloromethane</v>
-      </c>
-      <c r="CV493">
+        <v/>
+      </c>
+      <c r="CV493" t="str">
         <f t="shared" si="23"/>
-        <v>-3.77</v>
+        <v/>
       </c>
     </row>
     <row r="494" spans="1:100" x14ac:dyDescent="0.2">
@@ -52268,11 +52865,11 @@
       </c>
       <c r="CU494" t="str">
         <f t="shared" si="22"/>
-        <v>tetrafluoromethane</v>
-      </c>
-      <c r="CV494">
+        <v/>
+      </c>
+      <c r="CV494" t="str">
         <f t="shared" si="23"/>
-        <v>1.5</v>
+        <v/>
       </c>
     </row>
     <row r="495" spans="1:100" x14ac:dyDescent="0.2">
@@ -52363,11 +52960,11 @@
       </c>
       <c r="CU495" t="str">
         <f t="shared" si="22"/>
-        <v>tetrahydrofuran</v>
-      </c>
-      <c r="CV495">
+        <v/>
+      </c>
+      <c r="CV495" t="str">
         <f t="shared" si="23"/>
-        <v>-3.93</v>
+        <v/>
       </c>
     </row>
     <row r="496" spans="1:100" x14ac:dyDescent="0.2">
@@ -52461,11 +53058,11 @@
       </c>
       <c r="CU496" t="str">
         <f t="shared" si="22"/>
-        <v>tetrahydropyran</v>
-      </c>
-      <c r="CV496">
+        <v/>
+      </c>
+      <c r="CV496" t="str">
         <f t="shared" si="23"/>
-        <v>-4.21</v>
+        <v/>
       </c>
     </row>
     <row r="497" spans="1:100" x14ac:dyDescent="0.2">
@@ -52559,11 +53156,11 @@
       </c>
       <c r="CU497" t="str">
         <f t="shared" si="22"/>
-        <v>thiophene</v>
-      </c>
-      <c r="CV497">
+        <v/>
+      </c>
+      <c r="CV497" t="str">
         <f t="shared" si="23"/>
-        <v>-3.89</v>
+        <v/>
       </c>
     </row>
     <row r="498" spans="1:100" x14ac:dyDescent="0.2">
@@ -52663,11 +53260,11 @@
       </c>
       <c r="CU498" t="str">
         <f t="shared" si="22"/>
-        <v>thiophenol</v>
-      </c>
-      <c r="CV498">
+        <v/>
+      </c>
+      <c r="CV498" t="str">
         <f t="shared" si="23"/>
-        <v>-5.99</v>
+        <v/>
       </c>
     </row>
     <row r="499" spans="1:100" x14ac:dyDescent="0.2">
@@ -52912,7 +53509,7 @@
       </c>
       <c r="CV499">
         <f t="shared" si="23"/>
-        <v>-4.55</v>
+        <v>-4.88</v>
       </c>
     </row>
     <row r="500" spans="1:100" x14ac:dyDescent="0.2">
@@ -53187,11 +53784,11 @@
       </c>
       <c r="CU502" t="str">
         <f t="shared" si="22"/>
-        <v>tribromomethane</v>
-      </c>
-      <c r="CV502">
+        <v/>
+      </c>
+      <c r="CV502" t="str">
         <f t="shared" si="23"/>
-        <v>-5.62</v>
+        <v/>
       </c>
     </row>
     <row r="503" spans="1:100" x14ac:dyDescent="0.2">
@@ -53288,11 +53885,11 @@
       </c>
       <c r="CU503" t="str">
         <f t="shared" si="22"/>
-        <v>trichloroethene</v>
-      </c>
-      <c r="CV503">
+        <v/>
+      </c>
+      <c r="CV503" t="str">
         <f t="shared" si="23"/>
-        <v>-3.75</v>
+        <v/>
       </c>
     </row>
     <row r="504" spans="1:100" x14ac:dyDescent="0.2">
@@ -53404,11 +54001,11 @@
       </c>
       <c r="CU504" t="str">
         <f t="shared" si="22"/>
-        <v>trichloromethane</v>
-      </c>
-      <c r="CV504">
+        <v/>
+      </c>
+      <c r="CV504" t="str">
         <f t="shared" si="23"/>
-        <v>-3.81</v>
+        <v/>
       </c>
     </row>
     <row r="505" spans="1:100" x14ac:dyDescent="0.2">
@@ -53514,11 +54111,11 @@
       </c>
       <c r="CU505" t="str">
         <f t="shared" si="22"/>
-        <v>triethyl_phosphate</v>
-      </c>
-      <c r="CV505">
+        <v/>
+      </c>
+      <c r="CV505" t="str">
         <f t="shared" si="23"/>
-        <v>-8.8800000000000008</v>
+        <v/>
       </c>
     </row>
     <row r="506" spans="1:100" x14ac:dyDescent="0.2">
@@ -53631,7 +54228,7 @@
       </c>
       <c r="CV506">
         <f t="shared" si="23"/>
-        <v>-5.19</v>
+        <v>-3.76</v>
       </c>
     </row>
     <row r="507" spans="1:100" x14ac:dyDescent="0.2">
@@ -53906,11 +54503,11 @@
       </c>
       <c r="CU509" t="str">
         <f t="shared" si="22"/>
-        <v>trimethyl_phosphate</v>
-      </c>
-      <c r="CV509">
+        <v/>
+      </c>
+      <c r="CV509" t="str">
         <f t="shared" si="23"/>
-        <v>-7.81</v>
+        <v/>
       </c>
     </row>
     <row r="510" spans="1:100" x14ac:dyDescent="0.2">
@@ -54047,7 +54644,7 @@
       </c>
       <c r="CV510">
         <f t="shared" si="23"/>
-        <v>-3.6</v>
+        <v>-0.82</v>
       </c>
     </row>
     <row r="511" spans="1:100" x14ac:dyDescent="0.2">
@@ -67735,10 +68332,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P432"/>
+  <dimension ref="A1:Q432"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -67748,46 +68345,48 @@
     <col min="8" max="11" width="11.33203125" style="3" customWidth="1"/>
     <col min="12" max="12" width="13.6640625" style="3" customWidth="1"/>
     <col min="13" max="15" width="11.33203125" style="3" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="17" max="17" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="11" t="s">
         <v>78</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="11" t="s">
         <v>92</v>
       </c>
       <c r="N1" s="3" t="s">
@@ -67797,7 +68396,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>346</v>
       </c>
@@ -67846,8 +68445,11 @@
       <c r="P2">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q2" s="8" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>361</v>
       </c>
@@ -67896,8 +68498,11 @@
       <c r="P3">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q3" s="12" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>431</v>
       </c>
@@ -67946,8 +68551,11 @@
       <c r="P4">
         <v>14</v>
       </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q4" s="10" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>446</v>
       </c>
@@ -67996,8 +68604,11 @@
       <c r="P5">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="Q5" s="9" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>511</v>
       </c>
@@ -68047,8 +68658,8 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="3">
@@ -68094,7 +68705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>362</v>
       </c>
@@ -68141,8 +68752,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B9" s="3">
@@ -68188,7 +68799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>447</v>
       </c>
@@ -68236,8 +68847,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="9" t="s">
         <v>145</v>
       </c>
       <c r="B11" s="3">
@@ -68283,7 +68894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>94</v>
       </c>
@@ -68330,7 +68941,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>558</v>
       </c>
@@ -68377,7 +68988,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>71</v>
       </c>
@@ -68424,8 +69035,8 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A15" s="7" t="s">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="9" t="s">
         <v>88</v>
       </c>
       <c r="C15" s="4">
@@ -68465,8 +69076,8 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="9" t="s">
         <v>84</v>
       </c>
       <c r="C16" s="4">
@@ -68671,7 +69282,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
+      <c r="A21" s="9" t="s">
         <v>554</v>
       </c>
       <c r="C21" s="4">
@@ -68727,7 +69338,7 @@
       <c r="F22" s="3">
         <v>-12.44</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H22" s="5">
         <v>-13.67</v>
       </c>
       <c r="I22" s="3">
@@ -76310,4 +76921,438 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.1640625" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" customWidth="1"/>
+    <col min="13" max="13" width="22" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>597</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>614</v>
+      </c>
+      <c r="M1" s="3"/>
+    </row>
+    <row r="2" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>598</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0.69493611320516002</v>
+      </c>
+      <c r="C2" s="3">
+        <v>-31.998626554886101</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.12931089321622699</v>
+      </c>
+      <c r="E2" s="14">
+        <v>-5.1892651089931602E-2</v>
+      </c>
+      <c r="F2" s="3">
+        <v>-0.73390624614810296</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3.1237887733444299E-3</v>
+      </c>
+      <c r="H2" s="3">
+        <v>1.7175808308453699</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.71221199290794</v>
+      </c>
+      <c r="J2" s="3">
+        <v>1.85</v>
+      </c>
+      <c r="K2" s="15">
+        <v>78.36</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="B3" s="3">
+        <v>0.366741566047593</v>
+      </c>
+      <c r="C3" s="3">
+        <v>-41.197012551517702</v>
+      </c>
+      <c r="D3" s="3">
+        <v>-0.33339445977471799</v>
+      </c>
+      <c r="E3" s="3">
+        <v>-0.181399364335325</v>
+      </c>
+      <c r="F3" s="3">
+        <v>-0.40294760446393202</v>
+      </c>
+      <c r="G3" s="3">
+        <v>-1.2027233581941601E-2</v>
+      </c>
+      <c r="H3" s="4">
+        <v>1.9852665825817399</v>
+      </c>
+      <c r="I3" s="16">
+        <v>2.4952665428151199</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="K3" s="15">
+        <v>10.3</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>602</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0.27649257911035102</v>
+      </c>
+      <c r="C4" s="3">
+        <v>-16.480792820799401</v>
+      </c>
+      <c r="D4" s="3">
+        <v>-0.26410276929384402</v>
+      </c>
+      <c r="E4" s="3">
+        <v>-0.41646025236137002</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.33714285112926</v>
+      </c>
+      <c r="G4" s="3">
+        <v>-1.6822129154929699E-2</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.99944992936959</v>
+      </c>
+      <c r="I4" s="16">
+        <v>2.4650759773079498</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1.83</v>
+      </c>
+      <c r="K4" s="15">
+        <v>10.125</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>604</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0.16725590663298201</v>
+      </c>
+      <c r="C5" s="3">
+        <v>-39.116868176150597</v>
+      </c>
+      <c r="D5" s="3">
+        <v>-1.1142592618937099</v>
+      </c>
+      <c r="E5" s="3">
+        <v>-0.52638423147157898</v>
+      </c>
+      <c r="F5" s="3">
+        <v>-0.753770345323726</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-1.6777502413380802E-2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.99987047558589</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1.29174768093409</v>
+      </c>
+      <c r="J5" s="3">
+        <v>2.88</v>
+      </c>
+      <c r="K5" s="15">
+        <v>20.83</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>606</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0.232812336577575</v>
+      </c>
+      <c r="C6" s="3">
+        <v>-25.9097224181759</v>
+      </c>
+      <c r="D6" s="3">
+        <v>-0.85275581805063105</v>
+      </c>
+      <c r="E6" s="3">
+        <v>-0.45486269863883999</v>
+      </c>
+      <c r="F6" s="3">
+        <v>-0.13142848883410799</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-1.3933904999053601E-2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>1.99999999962084</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1.4599557779296699</v>
+      </c>
+      <c r="J6" s="3">
+        <v>3.96</v>
+      </c>
+      <c r="K6" s="15">
+        <v>48.826000000000001</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>608</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0.64866218444365498</v>
+      </c>
+      <c r="C7" s="3">
+        <v>-35.756640112848899</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.40063170947712101</v>
+      </c>
+      <c r="E7" s="14">
+        <v>-4.7448123028945299E-2</v>
+      </c>
+      <c r="F7" s="3">
+        <v>-0.64303038515179101</v>
+      </c>
+      <c r="G7" s="3">
+        <v>-1.4145557451559401E-2</v>
+      </c>
+      <c r="H7" s="4">
+        <v>1.99995610433869</v>
+      </c>
+      <c r="I7" s="3">
+        <v>1.81153319130216</v>
+      </c>
+      <c r="J7" s="3">
+        <v>1.68</v>
+      </c>
+      <c r="K7" s="15">
+        <v>20.523</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="B8" s="3">
+        <v>0.31691789413965799</v>
+      </c>
+      <c r="C8" s="3">
+        <v>-16.162387081048202</v>
+      </c>
+      <c r="D8" s="3">
+        <v>-0.711376366811028</v>
+      </c>
+      <c r="E8" s="3">
+        <v>-0.54296277539714899</v>
+      </c>
+      <c r="F8" s="3">
+        <v>-1.1233937241997001</v>
+      </c>
+      <c r="G8" s="3">
+        <v>-1.6199855506631299E-2</v>
+      </c>
+      <c r="H8" s="4">
+        <v>1.99527737981794</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1.6660055607158599</v>
+      </c>
+      <c r="J8" s="3">
+        <v>3.82</v>
+      </c>
+      <c r="K8" s="15">
+        <v>37.219000000000001</v>
+      </c>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0.74628172065768705</v>
+      </c>
+      <c r="C9" s="3">
+        <v>-20.336132102590899</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.49957647915710701</v>
+      </c>
+      <c r="E9" s="14">
+        <v>4.4366222911706103E-2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>1.45554911286639</v>
+      </c>
+      <c r="G9" s="3">
+        <v>-1.4115052596990099E-2</v>
+      </c>
+      <c r="H9" s="4">
+        <v>1.99954721620319</v>
+      </c>
+      <c r="I9" s="3">
+        <v>1.58795750691306</v>
+      </c>
+      <c r="J9" s="3">
+        <v>1.69</v>
+      </c>
+      <c r="K9" s="15">
+        <v>24.852</v>
+      </c>
+      <c r="M9" s="3"/>
+    </row>
+    <row r="10" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.76114121818119895</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-26.555254833616299</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.42907824856632398</v>
+      </c>
+      <c r="E10" s="14">
+        <v>7.0352514043804396E-2</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.49880092355129502</v>
+      </c>
+      <c r="G10" s="3">
+        <v>-1.32024315865355E-2</v>
+      </c>
+      <c r="H10" s="4">
+        <v>1.9996405233610099</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1.9424901312837</v>
+      </c>
+      <c r="J10" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="K10" s="15">
+        <v>32.613</v>
+      </c>
+      <c r="M10" s="3"/>
+    </row>
+    <row r="11" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>613</v>
+      </c>
+      <c r="B11" s="3">
+        <v>0.41806895920632098</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-15.863552178071499</v>
+      </c>
+      <c r="D11" s="3">
+        <v>-8.7002006227355502E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>-0.47867980967046297</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.870424223088891</v>
+      </c>
+      <c r="G11" s="3">
+        <v>-1.47284826286306E-2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>1.7770335089211799</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1.3075475819267</v>
+      </c>
+      <c r="J11" s="3">
+        <v>3.92</v>
+      </c>
+      <c r="K11" s="15">
+        <v>35.688000000000002</v>
+      </c>
+      <c r="M11" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Butanol results and modified paramNitromethane
</commit_message>
<xml_diff>
--- a/mobley/mnsol/Fulldata.xlsx
+++ b/mobley/mnsol/Fulldata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="1180" windowWidth="24960" windowHeight="13900" tabRatio="500"/>
+    <workbookView xWindow="220" yWindow="1180" windowWidth="24960" windowHeight="13900" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13218" uniqueCount="615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13220" uniqueCount="617">
   <si>
     <t>Compound</t>
   </si>
@@ -1878,6 +1878,12 @@
   <si>
     <t>geometry</t>
   </si>
+  <si>
+    <t>Butanol</t>
+  </si>
+  <si>
+    <t>Butanol shows the same trend as other alkanols for alpha (alpha decreases as MM of alkanol increases)</t>
+  </si>
 </sst>
 </file>
 
@@ -2004,7 +2010,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2041,6 +2047,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -2514,6 +2526,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>44823</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>44824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1329764</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>423543</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10040470" y="7156824"/>
+          <a:ext cx="1284941" cy="378719"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2782,7 +2838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CV514"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CP1" workbookViewId="0">
+    <sheetView topLeftCell="CP1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A505" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="CU2" sqref="CU2:CV513"/>
     </sheetView>
@@ -55326,7 +55382,7 @@
   <dimension ref="A1:P514"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A201" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -76929,10 +76985,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -76941,7 +76997,8 @@
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
     <col min="10" max="10" width="14.83203125" customWidth="1"/>
     <col min="12" max="12" width="17.83203125" customWidth="1"/>
-    <col min="13" max="13" width="22" customWidth="1"/>
+    <col min="13" max="13" width="52.33203125" customWidth="1"/>
+    <col min="14" max="14" width="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
@@ -77245,7 +77302,9 @@
       <c r="K8" s="15">
         <v>37.219000000000001</v>
       </c>
-      <c r="M8" s="3"/>
+      <c r="M8" s="18" t="s">
+        <v>616</v>
+      </c>
     </row>
     <row r="9" spans="1:13" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
@@ -77354,6 +77413,38 @@
         <v>35.688000000000002</v>
       </c>
       <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>615</v>
+      </c>
+      <c r="B12" s="13">
+        <v>0.56786769753029698</v>
+      </c>
+      <c r="C12" s="3">
+        <v>-77.510629762558494</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.98759259242481301</v>
+      </c>
+      <c r="E12" s="14">
+        <v>-1.0283499999999999E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.84762199992024401</v>
+      </c>
+      <c r="G12" s="3">
+        <v>-1.4813566560060601E-2</v>
+      </c>
+      <c r="H12" s="4">
+        <v>1.98039520145966</v>
+      </c>
+      <c r="I12" s="3">
+        <v>2.58</v>
+      </c>
+      <c r="K12" s="15">
+        <v>17.329999999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated Fulldata.xls, paramDMF and loadResults.m
</commit_message>
<xml_diff>
--- a/mobley/mnsol/Fulldata.xlsx
+++ b/mobley/mnsol/Fulldata.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="220" yWindow="700" windowWidth="24960" windowHeight="13900" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="220" yWindow="700" windowWidth="24960" windowHeight="13900" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="1" r:id="rId1"/>
-    <sheet name="Solvents_neutral" sheetId="2" r:id="rId2"/>
-    <sheet name="Solvents_neutral&amp;ions" sheetId="3" r:id="rId3"/>
-    <sheet name="Solvents_ions_only" sheetId="4" r:id="rId4"/>
-    <sheet name="consistent_set_neutral+ions" sheetId="5" r:id="rId5"/>
-    <sheet name="Results" sheetId="6" r:id="rId6"/>
+    <sheet name="Alkanes" sheetId="8" r:id="rId2"/>
+    <sheet name="Alkanols" sheetId="9" r:id="rId3"/>
+    <sheet name="Solvents_neutral" sheetId="2" r:id="rId4"/>
+    <sheet name="Solvents_neutral&amp;ions" sheetId="3" r:id="rId5"/>
+    <sheet name="Solvents_ions_only" sheetId="4" r:id="rId6"/>
+    <sheet name="consistent_set_neutral+ions" sheetId="5" r:id="rId7"/>
+    <sheet name="Results" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13239" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13298" uniqueCount="626">
   <si>
     <t>Compound</t>
   </si>
@@ -1816,9 +1818,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>RMS</t>
   </si>
   <si>
@@ -1910,6 +1909,9 @@
   </si>
   <si>
     <t>Dimethylacetamide</t>
+  </si>
+  <si>
+    <t>B [-2,2]</t>
   </si>
 </sst>
 </file>
@@ -2024,8 +2026,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2095,7 +2099,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2106,6 +2110,7 @@
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2116,6 +2121,7 @@
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2749,13 +2755,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>149410</xdr:colOff>
+      <xdr:colOff>134469</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>59764</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1210924</xdr:colOff>
+      <xdr:colOff>1195983</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>821764</xdr:rowOff>
     </xdr:to>
@@ -2780,7 +2786,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10145057" y="9203764"/>
+          <a:off x="10130116" y="9203764"/>
           <a:ext cx="1061514" cy="762000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -3056,11 +3062,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV514"/>
+  <dimension ref="A1:CV515"/>
   <sheetViews>
-    <sheetView topLeftCell="CK1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A494" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="CU2" sqref="CU2:CV513"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A522" sqref="A522"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3446,11 +3452,11 @@
         <v>1</v>
       </c>
       <c r="CU2" t="str">
-        <f>IF(ISNUMBER(CR2),A2,"")</f>
+        <f>IF(ISNUMBER(BS2),A2,"")</f>
         <v/>
       </c>
       <c r="CV2" t="str">
-        <f>IF(ISNUMBER(CR2),CR2,"")</f>
+        <f>IF(ISNUMBER(BS2),BS2,"")</f>
         <v/>
       </c>
     </row>
@@ -3535,11 +3541,11 @@
         <v>1</v>
       </c>
       <c r="CU3" t="str">
-        <f t="shared" ref="CU3:CU66" si="0">IF(ISNUMBER(CR3),A3,"")</f>
+        <f t="shared" ref="CU3:CU66" si="0">IF(ISNUMBER(BS3),A3,"")</f>
         <v/>
       </c>
       <c r="CV3" t="str">
-        <f t="shared" ref="CV3:CV66" si="1">IF(ISNUMBER(CR3),CR3,"")</f>
+        <f t="shared" ref="CV3:CV66" si="1">IF(ISNUMBER(BS3),BS3,"")</f>
         <v/>
       </c>
     </row>
@@ -9435,11 +9441,11 @@
         <v>1</v>
       </c>
       <c r="CU67" t="str">
-        <f t="shared" ref="CU67:CU130" si="4">IF(ISNUMBER(CR67),A67,"")</f>
+        <f t="shared" ref="CU67:CU130" si="4">IF(ISNUMBER(BS67),A67,"")</f>
         <v/>
       </c>
       <c r="CV67" t="str">
-        <f t="shared" ref="CV67:CV130" si="5">IF(ISNUMBER(CR67),CR67,"")</f>
+        <f t="shared" ref="CV67:CV130" si="5">IF(ISNUMBER(BS67),BS67,"")</f>
         <v/>
       </c>
     </row>
@@ -9648,11 +9654,11 @@
       </c>
       <c r="CU68" t="str">
         <f t="shared" si="4"/>
-        <v/>
-      </c>
-      <c r="CV68" t="str">
+        <v>14_dioxane</v>
+      </c>
+      <c r="CV68">
         <f t="shared" si="5"/>
-        <v/>
+        <v>-5.01</v>
       </c>
     </row>
     <row r="69" spans="1:100" x14ac:dyDescent="0.2">
@@ -15467,11 +15473,11 @@
         <v>1</v>
       </c>
       <c r="CU131" t="str">
-        <f t="shared" ref="CU131:CU194" si="7">IF(ISNUMBER(CR131),A131,"")</f>
+        <f t="shared" ref="CU131:CU194" si="7">IF(ISNUMBER(BS131),A131,"")</f>
         <v/>
       </c>
       <c r="CV131" t="str">
-        <f t="shared" ref="CV131:CV194" si="8">IF(ISNUMBER(CR131),CR131,"")</f>
+        <f t="shared" ref="CV131:CV194" si="8">IF(ISNUMBER(BS131),BS131,"")</f>
         <v/>
       </c>
     </row>
@@ -21457,11 +21463,11 @@
         <v>1</v>
       </c>
       <c r="CU195" t="str">
-        <f t="shared" ref="CU195:CU258" si="10">IF(ISNUMBER(CR195),A195,"")</f>
+        <f t="shared" ref="CU195:CU258" si="10">IF(ISNUMBER(BS195),A195,"")</f>
         <v/>
       </c>
       <c r="CV195" t="str">
-        <f t="shared" ref="CV195:CV258" si="11">IF(ISNUMBER(CR195),CR195,"")</f>
+        <f t="shared" ref="CV195:CV258" si="11">IF(ISNUMBER(BS195),BS195,"")</f>
         <v/>
       </c>
     </row>
@@ -22691,11 +22697,11 @@
       </c>
       <c r="CU207" t="str">
         <f t="shared" si="10"/>
-        <v>acetic_acid</v>
-      </c>
-      <c r="CV207">
+        <v/>
+      </c>
+      <c r="CV207" t="str">
         <f t="shared" si="11"/>
-        <v>-4.78</v>
+        <v/>
       </c>
     </row>
     <row r="208" spans="1:100" x14ac:dyDescent="0.2">
@@ -23212,11 +23218,11 @@
       </c>
       <c r="CU211" t="str">
         <f t="shared" si="10"/>
-        <v>aniline</v>
-      </c>
-      <c r="CV211">
+        <v/>
+      </c>
+      <c r="CV211" t="str">
         <f t="shared" si="11"/>
-        <v>-7.15</v>
+        <v/>
       </c>
     </row>
     <row r="212" spans="1:100" x14ac:dyDescent="0.2">
@@ -24825,7 +24831,7 @@
       </c>
       <c r="CV225">
         <f t="shared" si="11"/>
-        <v>-62.140999999999998</v>
+        <v>-55.927342260000003</v>
       </c>
     </row>
     <row r="226" spans="1:100" x14ac:dyDescent="0.2">
@@ -26138,11 +26144,11 @@
       </c>
       <c r="CU237" t="str">
         <f t="shared" si="10"/>
-        <v>butanoic_acid</v>
-      </c>
-      <c r="CV237">
+        <v/>
+      </c>
+      <c r="CV237" t="str">
         <f t="shared" si="11"/>
-        <v>-5.84</v>
+        <v/>
       </c>
     </row>
     <row r="238" spans="1:100" x14ac:dyDescent="0.2">
@@ -26380,11 +26386,11 @@
       </c>
       <c r="CU238" t="str">
         <f t="shared" si="10"/>
-        <v/>
-      </c>
-      <c r="CV238" t="str">
+        <v>butanone</v>
+      </c>
+      <c r="CV238">
         <f t="shared" si="11"/>
-        <v/>
+        <v>-4.5199999999999996</v>
       </c>
     </row>
     <row r="239" spans="1:100" x14ac:dyDescent="0.2">
@@ -27305,7 +27311,7 @@
       </c>
       <c r="CV247">
         <f t="shared" si="11"/>
-        <v>-65.727000000000004</v>
+        <v>-59.536328869999998</v>
       </c>
     </row>
     <row r="248" spans="1:100" x14ac:dyDescent="0.2">
@@ -27436,7 +27442,7 @@
       </c>
       <c r="CV248">
         <f t="shared" si="11"/>
-        <v>-69.551000000000002</v>
+        <v>-74.808795410000002</v>
       </c>
     </row>
     <row r="249" spans="1:100" x14ac:dyDescent="0.2">
@@ -28488,11 +28494,11 @@
         <v>4</v>
       </c>
       <c r="CU259" t="str">
-        <f t="shared" ref="CU259:CU322" si="13">IF(ISNUMBER(CR259),A259,"")</f>
+        <f t="shared" ref="CU259:CU322" si="13">IF(ISNUMBER(BS259),A259,"")</f>
         <v/>
       </c>
       <c r="CV259" t="str">
-        <f t="shared" ref="CV259:CV322" si="14">IF(ISNUMBER(CR259),CR259,"")</f>
+        <f t="shared" ref="CV259:CV322" si="14">IF(ISNUMBER(BS259),BS259,"")</f>
         <v/>
       </c>
     </row>
@@ -32374,11 +32380,11 @@
       </c>
       <c r="CU298" t="str">
         <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="CV298" t="str">
+        <v>ethanol</v>
+      </c>
+      <c r="CV298">
         <f t="shared" si="14"/>
-        <v/>
+        <v>-5.4</v>
       </c>
     </row>
     <row r="299" spans="1:100" x14ac:dyDescent="0.2">
@@ -34985,11 +34991,11 @@
         <v>1</v>
       </c>
       <c r="CU323" t="str">
-        <f t="shared" ref="CU323:CU386" si="16">IF(ISNUMBER(CR323),A323,"")</f>
+        <f t="shared" ref="CU323:CU386" si="16">IF(ISNUMBER(BS323),A323,"")</f>
         <v/>
       </c>
       <c r="CV323" t="str">
-        <f t="shared" ref="CV323:CV386" si="17">IF(ISNUMBER(CR323),CR323,"")</f>
+        <f t="shared" ref="CV323:CV386" si="17">IF(ISNUMBER(BS323),BS323,"")</f>
         <v/>
       </c>
     </row>
@@ -35685,11 +35691,11 @@
       </c>
       <c r="CU329" t="str">
         <f t="shared" si="16"/>
-        <v>hexanoic_acid</v>
-      </c>
-      <c r="CV329">
+        <v/>
+      </c>
+      <c r="CV329" t="str">
         <f t="shared" si="17"/>
-        <v>-7.26</v>
+        <v/>
       </c>
     </row>
     <row r="330" spans="1:100" x14ac:dyDescent="0.2">
@@ -36019,7 +36025,7 @@
       </c>
       <c r="CV332">
         <f t="shared" si="17"/>
-        <v>-63.576000000000001</v>
+        <v>-53.059273419999997</v>
       </c>
     </row>
     <row r="333" spans="1:100" x14ac:dyDescent="0.2">
@@ -37756,7 +37762,7 @@
       </c>
       <c r="CV350">
         <f t="shared" si="17"/>
-        <v>-78.632999999999996</v>
+        <v>-86.926386230000006</v>
       </c>
     </row>
     <row r="351" spans="1:100" x14ac:dyDescent="0.2">
@@ -37884,7 +37890,7 @@
       </c>
       <c r="CV351">
         <f t="shared" si="17"/>
-        <v>-117.352</v>
+        <v>-131.69216059999999</v>
       </c>
     </row>
     <row r="352" spans="1:100" x14ac:dyDescent="0.2">
@@ -38112,11 +38118,11 @@
       </c>
       <c r="CU353" t="str">
         <f t="shared" si="16"/>
-        <v>m_cresol</v>
-      </c>
-      <c r="CV353">
+        <v/>
+      </c>
+      <c r="CV353" t="str">
         <f t="shared" si="17"/>
-        <v>-7.29</v>
+        <v/>
       </c>
     </row>
     <row r="354" spans="1:100" x14ac:dyDescent="0.2">
@@ -38698,11 +38704,11 @@
       </c>
       <c r="CU358" t="str">
         <f t="shared" si="16"/>
-        <v>methanol</v>
-      </c>
-      <c r="CV358">
+        <v/>
+      </c>
+      <c r="CV358" t="str">
         <f t="shared" si="17"/>
-        <v>-2.93</v>
+        <v/>
       </c>
     </row>
     <row r="359" spans="1:100" x14ac:dyDescent="0.2">
@@ -41575,11 +41581,11 @@
         <v>1</v>
       </c>
       <c r="CU387" t="str">
-        <f t="shared" ref="CU387:CU450" si="19">IF(ISNUMBER(CR387),A387,"")</f>
+        <f t="shared" ref="CU387:CU450" si="19">IF(ISNUMBER(BS387),A387,"")</f>
         <v/>
       </c>
       <c r="CV387" t="str">
-        <f t="shared" ref="CV387:CV450" si="20">IF(ISNUMBER(CR387),CR387,"")</f>
+        <f t="shared" ref="CV387:CV450" si="20">IF(ISNUMBER(BS387),BS387,"")</f>
         <v/>
       </c>
     </row>
@@ -44079,11 +44085,11 @@
       </c>
       <c r="CU410" t="str">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="CV410" t="str">
+        <v>n_octane</v>
+      </c>
+      <c r="CV410">
         <f t="shared" si="20"/>
-        <v/>
+        <v>-3.94</v>
       </c>
     </row>
     <row r="411" spans="1:100" x14ac:dyDescent="0.2">
@@ -45738,7 +45744,7 @@
       </c>
       <c r="CV426">
         <f t="shared" si="20"/>
-        <v>-93.212000000000003</v>
+        <v>-104.2304015</v>
       </c>
     </row>
     <row r="427" spans="1:100" x14ac:dyDescent="0.2">
@@ -46011,11 +46017,11 @@
       </c>
       <c r="CU428" t="str">
         <f t="shared" si="19"/>
-        <v>nitrobenzene</v>
-      </c>
-      <c r="CV428">
+        <v/>
+      </c>
+      <c r="CV428" t="str">
         <f t="shared" si="20"/>
-        <v>-7.94</v>
+        <v/>
       </c>
     </row>
     <row r="429" spans="1:100" x14ac:dyDescent="0.2">
@@ -46337,7 +46343,7 @@
       </c>
       <c r="CV430">
         <f t="shared" si="20"/>
-        <v>-4.9000000000000004</v>
+        <v>-5.62</v>
       </c>
     </row>
     <row r="431" spans="1:100" x14ac:dyDescent="0.2">
@@ -47390,11 +47396,11 @@
       </c>
       <c r="CU441" t="str">
         <f t="shared" si="19"/>
-        <v>o_cresol</v>
-      </c>
-      <c r="CV441">
+        <v/>
+      </c>
+      <c r="CV441" t="str">
         <f t="shared" si="20"/>
-        <v>-8.16</v>
+        <v/>
       </c>
     </row>
     <row r="442" spans="1:100" x14ac:dyDescent="0.2">
@@ -48234,11 +48240,11 @@
       </c>
       <c r="CU449" t="str">
         <f t="shared" si="19"/>
-        <v>p_cresol</v>
-      </c>
-      <c r="CV449">
+        <v/>
+      </c>
+      <c r="CV449" t="str">
         <f t="shared" si="20"/>
-        <v>-8.1300000000000008</v>
+        <v/>
       </c>
     </row>
     <row r="450" spans="1:100" x14ac:dyDescent="0.2">
@@ -48420,11 +48426,11 @@
         <v>4</v>
       </c>
       <c r="CU451" t="str">
-        <f t="shared" ref="CU451:CU513" si="22">IF(ISNUMBER(CR451),A451,"")</f>
+        <f t="shared" ref="CU451:CU513" si="22">IF(ISNUMBER(BS451),A451,"")</f>
         <v/>
       </c>
       <c r="CV451" t="str">
-        <f t="shared" ref="CV451:CV513" si="23">IF(ISNUMBER(CR451),CR451,"")</f>
+        <f t="shared" ref="CV451:CV513" si="23">IF(ISNUMBER(BS451),BS451,"")</f>
         <v/>
       </c>
     </row>
@@ -49809,11 +49815,11 @@
       </c>
       <c r="CU464" t="str">
         <f t="shared" si="22"/>
-        <v>pentanoic_acid</v>
-      </c>
-      <c r="CV464">
+        <v/>
+      </c>
+      <c r="CV464" t="str">
         <f t="shared" si="23"/>
-        <v>-6.47</v>
+        <v/>
       </c>
     </row>
     <row r="465" spans="1:100" x14ac:dyDescent="0.2">
@@ -50146,11 +50152,11 @@
       </c>
       <c r="CU466" t="str">
         <f t="shared" si="22"/>
-        <v>phenol</v>
-      </c>
-      <c r="CV466">
+        <v/>
+      </c>
+      <c r="CV466" t="str">
         <f t="shared" si="23"/>
-        <v>-7.86</v>
+        <v/>
       </c>
     </row>
     <row r="467" spans="1:100" x14ac:dyDescent="0.2">
@@ -51341,11 +51347,11 @@
       </c>
       <c r="CU477" t="str">
         <f t="shared" si="22"/>
-        <v>propanoic_acid</v>
-      </c>
-      <c r="CV477">
+        <v/>
+      </c>
+      <c r="CV477" t="str">
         <f t="shared" si="23"/>
-        <v>-5.38</v>
+        <v/>
       </c>
     </row>
     <row r="478" spans="1:100" x14ac:dyDescent="0.2">
@@ -52490,7 +52496,7 @@
       </c>
       <c r="CV487">
         <f t="shared" si="23"/>
-        <v>-74.091999999999999</v>
+        <v>-80.544933080000007</v>
       </c>
     </row>
     <row r="488" spans="1:100" x14ac:dyDescent="0.2">
@@ -53785,11 +53791,11 @@
       </c>
       <c r="CU499" t="str">
         <f t="shared" si="22"/>
-        <v/>
-      </c>
-      <c r="CV499" t="str">
+        <v>toluene</v>
+      </c>
+      <c r="CV499">
         <f t="shared" si="23"/>
-        <v/>
+        <v>-4.9400000000000004</v>
       </c>
     </row>
     <row r="500" spans="1:100" x14ac:dyDescent="0.2">
@@ -55578,6 +55584,380 @@
       <c r="CS514">
         <f>COUNT(CS2:CS513)</f>
         <v>14</v>
+      </c>
+    </row>
+    <row r="515" spans="1:100" x14ac:dyDescent="0.2">
+      <c r="B515" t="str">
+        <f>IF(B$514&gt;18,B$1,"")</f>
+        <v>xylene</v>
+      </c>
+      <c r="C515" t="str">
+        <f>IF(C$514&gt;18,C$1,"")</f>
+        <v/>
+      </c>
+      <c r="D515" t="str">
+        <f t="shared" ref="D515:O515" si="27">IF(D$514&gt;18,D$1,"")</f>
+        <v/>
+      </c>
+      <c r="E515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="F515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="G515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="H515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="I515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="J515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="K515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="L515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="M515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="N515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="O515" t="str">
+        <f t="shared" si="27"/>
+        <v/>
+      </c>
+      <c r="P515" t="str">
+        <f>IF(P$514&gt;18,P$1,"")</f>
+        <v/>
+      </c>
+      <c r="Q515" t="str">
+        <f>IF(Q$514&gt;18,Q$1,"")</f>
+        <v/>
+      </c>
+      <c r="R515" t="str">
+        <f t="shared" ref="R515:T515" si="28">IF(R$514&gt;18,R$1,"")</f>
+        <v>pentanol</v>
+      </c>
+      <c r="S515" t="str">
+        <f t="shared" si="28"/>
+        <v>pentane</v>
+      </c>
+      <c r="T515" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="U515" t="str">
+        <f>IF(U$514&gt;18,U$1,"")</f>
+        <v/>
+      </c>
+      <c r="V515" t="str">
+        <f>IF(V$514&gt;18,V$1,"")</f>
+        <v/>
+      </c>
+      <c r="W515" t="str">
+        <f t="shared" ref="W515:AB515" si="29">IF(W$514&gt;18,W$1,"")</f>
+        <v>octane</v>
+      </c>
+      <c r="X515" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="Y515" t="str">
+        <f t="shared" si="29"/>
+        <v>nonane</v>
+      </c>
+      <c r="Z515" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="AA515" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="AB515" t="str">
+        <f t="shared" si="29"/>
+        <v/>
+      </c>
+      <c r="AC515" t="str">
+        <f>IF(AC$514&gt;18,AC$1,"")</f>
+        <v/>
+      </c>
+      <c r="AD515" t="str">
+        <f>IF(AD$514&gt;18,AD$1,"")</f>
+        <v/>
+      </c>
+      <c r="AE515" t="str">
+        <f t="shared" ref="AE515:AH515" si="30">IF(AE$514&gt;18,AE$1,"")</f>
+        <v/>
+      </c>
+      <c r="AF515" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="AG515" t="str">
+        <f t="shared" si="30"/>
+        <v>isooctane</v>
+      </c>
+      <c r="AH515" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="AI515" t="str">
+        <f>IF(AI$514&gt;18,AI$1,"")</f>
+        <v>iodobenzene</v>
+      </c>
+      <c r="AJ515" t="str">
+        <f>IF(AJ$514&gt;18,AJ$1,"")</f>
+        <v/>
+      </c>
+      <c r="AK515" t="str">
+        <f t="shared" ref="AK515:AP515" si="31">IF(AK$514&gt;18,AK$1,"")</f>
+        <v/>
+      </c>
+      <c r="AL515" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="AM515" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="AN515" t="str">
+        <f t="shared" si="31"/>
+        <v>heptane</v>
+      </c>
+      <c r="AO515" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="AP515" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="AQ515" t="str">
+        <f>IF(AQ$514&gt;18,AQ$1,"")</f>
+        <v>ethylbenzene</v>
+      </c>
+      <c r="AR515" t="str">
+        <f>IF(AR$514&gt;18,AR$1,"")</f>
+        <v/>
+      </c>
+      <c r="AS515" t="str">
+        <f t="shared" ref="AS515" si="32">IF(AS$514&gt;18,AS$1,"")</f>
+        <v/>
+      </c>
+      <c r="AT515" t="str">
+        <f>IF(AT$514&gt;18,AT$1,"")</f>
+        <v/>
+      </c>
+      <c r="AU515" t="str">
+        <f>IF(AU$514&gt;18,AU$1,"")</f>
+        <v/>
+      </c>
+      <c r="AV515" t="str">
+        <f t="shared" ref="AV515:BB515" si="33">IF(AV$514&gt;18,AV$1,"")</f>
+        <v>diisopropylether</v>
+      </c>
+      <c r="AW515" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AX515" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AY515" t="str">
+        <f t="shared" si="33"/>
+        <v>decane</v>
+      </c>
+      <c r="AZ515" t="str">
+        <f t="shared" si="33"/>
+        <v>decalin</v>
+      </c>
+      <c r="BA515" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="BB515" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="BC515" t="str">
+        <f>IF(BC$514&gt;18,BC$1,"")</f>
+        <v>chlorobenzene</v>
+      </c>
+      <c r="BD515" t="str">
+        <f>IF(BD$514&gt;18,BD$1,"")</f>
+        <v/>
+      </c>
+      <c r="BE515" t="str">
+        <f t="shared" ref="BE515:BK515" si="34">IF(BE$514&gt;18,BE$1,"")</f>
+        <v/>
+      </c>
+      <c r="BF515" t="str">
+        <f t="shared" si="34"/>
+        <v>butylacetate</v>
+      </c>
+      <c r="BG515" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="BH515" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="BI515" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="BJ515" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="BK515" t="str">
+        <f t="shared" si="34"/>
+        <v>bromobenzene</v>
+      </c>
+      <c r="BL515" t="str">
+        <f>IF(BL$514&gt;18,BL$1,"")</f>
+        <v/>
+      </c>
+      <c r="BM515" t="str">
+        <f>IF(BM$514&gt;18,BM$1,"")</f>
+        <v/>
+      </c>
+      <c r="BN515" t="str">
+        <f t="shared" ref="BN515:BR515" si="35">IF(BN$514&gt;18,BN$1,"")</f>
+        <v/>
+      </c>
+      <c r="BO515" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="BP515" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="BQ515" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="BR515" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="BS515" t="str">
+        <f>IF(BS$514&gt;18,BS$1,"")</f>
+        <v/>
+      </c>
+      <c r="BT515" t="str">
+        <f>IF(BT$514&gt;18,BT$1,"")</f>
+        <v/>
+      </c>
+      <c r="BU515" t="str">
+        <f t="shared" ref="BU515:BZ515" si="36">IF(BU$514&gt;18,BU$1,"")</f>
+        <v>toluene</v>
+      </c>
+      <c r="BV515" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="BW515" t="str">
+        <f t="shared" si="36"/>
+        <v>hexane</v>
+      </c>
+      <c r="BX515" t="str">
+        <f t="shared" si="36"/>
+        <v>hexadecane</v>
+      </c>
+      <c r="BY515" t="str">
+        <f t="shared" si="36"/>
+        <v>carbontet</v>
+      </c>
+      <c r="BZ515" t="str">
+        <f t="shared" si="36"/>
+        <v>methanol</v>
+      </c>
+      <c r="CA515" t="str">
+        <f>IF(CA$514&gt;18,CA$1,"")</f>
+        <v>ethanol</v>
+      </c>
+      <c r="CB515" t="str">
+        <f>IF(CB$514&gt;18,CB$1,"")</f>
+        <v>propanol</v>
+      </c>
+      <c r="CC515" t="str">
+        <f t="shared" ref="CC515:CE515" si="37">IF(CC$514&gt;18,CC$1,"")</f>
+        <v>butanol</v>
+      </c>
+      <c r="CD515" t="str">
+        <f t="shared" si="37"/>
+        <v>dimethylofrmamide</v>
+      </c>
+      <c r="CE515" t="str">
+        <f t="shared" si="37"/>
+        <v>acetonitrile</v>
+      </c>
+      <c r="CF515" t="str">
+        <f>IF(CF$514&gt;18,CF$1,"")</f>
+        <v>dimethylsulfoxide</v>
+      </c>
+      <c r="CG515" t="str">
+        <f>IF(CG$514&gt;18,CG$1,"")</f>
+        <v>propanone</v>
+      </c>
+      <c r="CH515" t="str">
+        <f t="shared" ref="CH515:CL515" si="38">IF(CH$514&gt;18,CH$1,"")</f>
+        <v>cyclohexane</v>
+      </c>
+      <c r="CI515" t="str">
+        <f t="shared" si="38"/>
+        <v>diethylether</v>
+      </c>
+      <c r="CJ515" t="str">
+        <f t="shared" si="38"/>
+        <v>dibuthylether</v>
+      </c>
+      <c r="CK515" t="str">
+        <f t="shared" si="38"/>
+        <v>octanol</v>
+      </c>
+      <c r="CL515" t="str">
+        <f t="shared" si="38"/>
+        <v>benzene</v>
+      </c>
+      <c r="CM515" t="str">
+        <f>IF(CM$514&gt;18,CM$1,"")</f>
+        <v>chlorofom</v>
+      </c>
+      <c r="CN515" t="str">
+        <f>IF(CN$514&gt;18,CN$1,"")</f>
+        <v>12dichloroethane</v>
+      </c>
+      <c r="CO515" t="str">
+        <f>IF(CO$514&gt;18,CO$1,"")</f>
+        <v/>
+      </c>
+      <c r="CP515" t="str">
+        <f>IF(CP$514&gt;18,CP$1,"")</f>
+        <v>butylacetate</v>
       </c>
     </row>
   </sheetData>
@@ -55586,6 +55966,1069 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F1" t="s">
+        <v>49</v>
+      </c>
+      <c r="G1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B2">
+        <v>-4.43</v>
+      </c>
+      <c r="C2">
+        <v>-4.21</v>
+      </c>
+      <c r="D2">
+        <v>-4.1900000000000004</v>
+      </c>
+      <c r="E2">
+        <v>-4.3</v>
+      </c>
+      <c r="F2">
+        <v>-4.1500000000000004</v>
+      </c>
+      <c r="G2">
+        <v>-4.34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <v>-3.77</v>
+      </c>
+      <c r="C3">
+        <v>-3.69</v>
+      </c>
+      <c r="D3">
+        <v>-3.77</v>
+      </c>
+      <c r="E3">
+        <v>-3.66</v>
+      </c>
+      <c r="F3">
+        <v>-3.77</v>
+      </c>
+      <c r="G3">
+        <v>-3.77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4">
+        <v>-2.15</v>
+      </c>
+      <c r="C4">
+        <v>-2.15</v>
+      </c>
+      <c r="D4">
+        <v>-2.15</v>
+      </c>
+      <c r="E4">
+        <v>-2.15</v>
+      </c>
+      <c r="F4">
+        <v>-2.44</v>
+      </c>
+      <c r="G4">
+        <v>-2.73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>116</v>
+      </c>
+      <c r="B5">
+        <v>-3.69</v>
+      </c>
+      <c r="C5">
+        <v>-3.48</v>
+      </c>
+      <c r="D5">
+        <v>-3.45</v>
+      </c>
+      <c r="E5">
+        <v>-3.5</v>
+      </c>
+      <c r="F5">
+        <v>-3.43</v>
+      </c>
+      <c r="G5">
+        <v>-3.62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6">
+        <v>-2.1800000000000002</v>
+      </c>
+      <c r="C6">
+        <v>-2.04</v>
+      </c>
+      <c r="D6">
+        <v>-1.98</v>
+      </c>
+      <c r="E6">
+        <v>-2.09</v>
+      </c>
+      <c r="F6">
+        <v>-1.92</v>
+      </c>
+      <c r="G6">
+        <v>-2.09</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7">
+        <v>-5.62</v>
+      </c>
+      <c r="C7">
+        <v>-5.56</v>
+      </c>
+      <c r="D7">
+        <v>-5.62</v>
+      </c>
+      <c r="E7">
+        <v>-5.6</v>
+      </c>
+      <c r="F7">
+        <v>-5.62</v>
+      </c>
+      <c r="G7">
+        <v>-5.75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8">
+        <v>-5.4</v>
+      </c>
+      <c r="C8">
+        <v>-5.25</v>
+      </c>
+      <c r="D8">
+        <v>-5.24</v>
+      </c>
+      <c r="E8">
+        <v>-5.22</v>
+      </c>
+      <c r="F8">
+        <v>-5.18</v>
+      </c>
+      <c r="G8">
+        <v>-5.36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9">
+        <v>-4.97</v>
+      </c>
+      <c r="C9">
+        <v>-4.8600000000000003</v>
+      </c>
+      <c r="D9">
+        <v>-4.97</v>
+      </c>
+      <c r="E9">
+        <v>-4.8899999999999997</v>
+      </c>
+      <c r="F9">
+        <v>-4.97</v>
+      </c>
+      <c r="G9">
+        <v>-5.14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>126</v>
+      </c>
+      <c r="B10">
+        <v>-4.79</v>
+      </c>
+      <c r="C10">
+        <v>-4.5999999999999996</v>
+      </c>
+      <c r="D10">
+        <v>-4.59</v>
+      </c>
+      <c r="E10">
+        <v>-4.55</v>
+      </c>
+      <c r="F10">
+        <v>-4.6100000000000003</v>
+      </c>
+      <c r="G10">
+        <v>-4.68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="B11">
+        <v>-1.29</v>
+      </c>
+      <c r="C11">
+        <v>-1.29</v>
+      </c>
+      <c r="D11">
+        <v>-1.29</v>
+      </c>
+      <c r="E11">
+        <v>-1.29</v>
+      </c>
+      <c r="F11">
+        <v>-1.29</v>
+      </c>
+      <c r="G11">
+        <v>-1.49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>135</v>
+      </c>
+      <c r="B12">
+        <v>-5.67</v>
+      </c>
+      <c r="C12">
+        <v>-5.53</v>
+      </c>
+      <c r="D12">
+        <v>-5.51</v>
+      </c>
+      <c r="E12">
+        <v>-5.63</v>
+      </c>
+      <c r="F12">
+        <v>-5.48</v>
+      </c>
+      <c r="G12">
+        <v>-5.64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>137</v>
+      </c>
+      <c r="B13">
+        <v>-4.96</v>
+      </c>
+      <c r="C13">
+        <v>-4.8600000000000003</v>
+      </c>
+      <c r="D13">
+        <v>-4.8499999999999996</v>
+      </c>
+      <c r="E13">
+        <v>-4.92</v>
+      </c>
+      <c r="F13">
+        <v>-4.7699999999999996</v>
+      </c>
+      <c r="G13">
+        <v>-4.9400000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14">
+        <v>-3.69</v>
+      </c>
+      <c r="C14">
+        <v>-3.57</v>
+      </c>
+      <c r="D14">
+        <v>-3.5</v>
+      </c>
+      <c r="E14">
+        <v>-3.63</v>
+      </c>
+      <c r="F14">
+        <v>-3.49</v>
+      </c>
+      <c r="G14">
+        <v>-3.65</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15">
+        <v>-4.88</v>
+      </c>
+      <c r="C15">
+        <v>-4.8</v>
+      </c>
+      <c r="D15">
+        <v>-4.6900000000000004</v>
+      </c>
+      <c r="E15">
+        <v>-4.83</v>
+      </c>
+      <c r="F15">
+        <v>-4.66</v>
+      </c>
+      <c r="G15">
+        <v>-4.8600000000000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>147</v>
+      </c>
+      <c r="B16">
+        <v>-4.21</v>
+      </c>
+      <c r="C16">
+        <v>-4.09</v>
+      </c>
+      <c r="D16">
+        <v>-4.07</v>
+      </c>
+      <c r="E16">
+        <v>-4.09</v>
+      </c>
+      <c r="F16">
+        <v>-4.0199999999999996</v>
+      </c>
+      <c r="G16">
+        <v>-4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>149</v>
+      </c>
+      <c r="B17">
+        <v>-3.13</v>
+      </c>
+      <c r="C17">
+        <v>-3</v>
+      </c>
+      <c r="D17">
+        <v>-2.96</v>
+      </c>
+      <c r="E17">
+        <v>-3.03</v>
+      </c>
+      <c r="F17">
+        <v>-2.96</v>
+      </c>
+      <c r="G17">
+        <v>-3.13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B18">
+        <v>-3.92</v>
+      </c>
+      <c r="C18">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="D18">
+        <v>-3.92</v>
+      </c>
+      <c r="E18">
+        <v>-4.09</v>
+      </c>
+      <c r="F18">
+        <v>-3.92</v>
+      </c>
+      <c r="G18">
+        <v>-4.38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19">
+        <v>-2.76</v>
+      </c>
+      <c r="C19">
+        <v>-2.76</v>
+      </c>
+      <c r="D19">
+        <v>-2.76</v>
+      </c>
+      <c r="E19">
+        <v>-3.01</v>
+      </c>
+      <c r="F19">
+        <v>-2.76</v>
+      </c>
+      <c r="G19">
+        <v>-2.81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2">
+        <v>-13.21</v>
+      </c>
+      <c r="C2">
+        <v>-12.93</v>
+      </c>
+      <c r="D2">
+        <v>-12.63</v>
+      </c>
+      <c r="E2">
+        <v>-12.44</v>
+      </c>
+      <c r="F2">
+        <v>-11.35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B3">
+        <v>-10.48</v>
+      </c>
+      <c r="C3">
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="D3">
+        <v>-9.85</v>
+      </c>
+      <c r="E3">
+        <v>-9.7899999999999991</v>
+      </c>
+      <c r="F3">
+        <v>-10.47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B4">
+        <v>-3.76</v>
+      </c>
+      <c r="C4">
+        <v>-3.79</v>
+      </c>
+      <c r="D4">
+        <v>-3.79</v>
+      </c>
+      <c r="E4">
+        <v>-3.39</v>
+      </c>
+      <c r="F4">
+        <v>-3.72</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B5">
+        <v>-63.814999999999998</v>
+      </c>
+      <c r="C5">
+        <v>-62.094000000000001</v>
+      </c>
+      <c r="D5">
+        <v>-61.17</v>
+      </c>
+      <c r="E5">
+        <v>-60.75</v>
+      </c>
+      <c r="F5">
+        <v>-62.61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6">
+        <v>-6.35</v>
+      </c>
+      <c r="C6">
+        <v>-6.35</v>
+      </c>
+      <c r="D6">
+        <v>-6.1</v>
+      </c>
+      <c r="E6">
+        <v>-6.03</v>
+      </c>
+      <c r="F6">
+        <v>-5.71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7">
+        <v>-4.55</v>
+      </c>
+      <c r="C7">
+        <v>-4.32</v>
+      </c>
+      <c r="D7">
+        <v>-4.1500000000000004</v>
+      </c>
+      <c r="E7">
+        <v>-4.12</v>
+      </c>
+      <c r="F7">
+        <v>-3.78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>361</v>
+      </c>
+      <c r="B8">
+        <v>-69.551000000000002</v>
+      </c>
+      <c r="C8">
+        <v>-67.83</v>
+      </c>
+      <c r="D8">
+        <v>-66.61</v>
+      </c>
+      <c r="E8">
+        <v>-65.73</v>
+      </c>
+      <c r="F8">
+        <v>-68.19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>362</v>
+      </c>
+      <c r="B9">
+        <v>-70.984999999999999</v>
+      </c>
+      <c r="C9">
+        <v>-69.551000000000002</v>
+      </c>
+      <c r="D9">
+        <v>-68.930000000000007</v>
+      </c>
+      <c r="E9">
+        <v>-68.67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10">
+        <v>-3.47</v>
+      </c>
+      <c r="C10">
+        <v>-3.47</v>
+      </c>
+      <c r="D10">
+        <v>-3.47</v>
+      </c>
+      <c r="E10">
+        <v>-3.5</v>
+      </c>
+      <c r="F10">
+        <v>-3.46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>405</v>
+      </c>
+      <c r="B11">
+        <v>-0.59</v>
+      </c>
+      <c r="C11">
+        <v>-0.59</v>
+      </c>
+      <c r="D11">
+        <v>-0.61</v>
+      </c>
+      <c r="E11">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="F11">
+        <v>-0.64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B12">
+        <v>-4.9800000000000004</v>
+      </c>
+      <c r="C12">
+        <v>-5.04</v>
+      </c>
+      <c r="D12">
+        <v>-5.01</v>
+      </c>
+      <c r="E12">
+        <v>-5.0199999999999996</v>
+      </c>
+      <c r="F12">
+        <v>-4.3600000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>446</v>
+      </c>
+      <c r="B13">
+        <v>-81.739999999999995</v>
+      </c>
+      <c r="C13">
+        <v>-80.209999999999994</v>
+      </c>
+      <c r="D13">
+        <v>-79.86</v>
+      </c>
+      <c r="E13">
+        <v>-79.37</v>
+      </c>
+      <c r="F13">
+        <v>-80.930000000000007</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>447</v>
+      </c>
+      <c r="B14">
+        <v>-125.47799999999999</v>
+      </c>
+      <c r="C14">
+        <v>-123.80500000000001</v>
+      </c>
+      <c r="D14">
+        <v>-123.7</v>
+      </c>
+      <c r="F14">
+        <v>-123.89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15">
+        <v>-4.6100000000000003</v>
+      </c>
+      <c r="C15">
+        <v>-4.6399999999999997</v>
+      </c>
+      <c r="D15">
+        <v>-4.3</v>
+      </c>
+      <c r="E15">
+        <v>-4.7300000000000004</v>
+      </c>
+      <c r="F15">
+        <v>-3.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>479</v>
+      </c>
+      <c r="B16">
+        <v>-1.74</v>
+      </c>
+      <c r="C16">
+        <v>-1.91</v>
+      </c>
+      <c r="D16">
+        <v>-1.98</v>
+      </c>
+      <c r="E16">
+        <v>-1.96</v>
+      </c>
+      <c r="F16">
+        <v>-1.86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>485</v>
+      </c>
+      <c r="B17">
+        <v>-3.35</v>
+      </c>
+      <c r="C17">
+        <v>-3.69</v>
+      </c>
+      <c r="D17">
+        <v>-3.73</v>
+      </c>
+      <c r="E17">
+        <v>-3.87</v>
+      </c>
+      <c r="F17">
+        <v>-3.74</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>487</v>
+      </c>
+      <c r="B18">
+        <v>-2.8</v>
+      </c>
+      <c r="C18">
+        <v>-3.05</v>
+      </c>
+      <c r="D18">
+        <v>-3.1</v>
+      </c>
+      <c r="E18">
+        <v>-3.31</v>
+      </c>
+      <c r="F18">
+        <v>-3.01</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>145</v>
+      </c>
+      <c r="B19">
+        <v>-4.3</v>
+      </c>
+      <c r="C19">
+        <v>-4.2300000000000004</v>
+      </c>
+      <c r="D19">
+        <v>-4.3899999999999997</v>
+      </c>
+      <c r="E19">
+        <v>-4.45</v>
+      </c>
+      <c r="F19">
+        <v>-4.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>499</v>
+      </c>
+      <c r="B20">
+        <v>-2.27</v>
+      </c>
+      <c r="C20">
+        <v>-2.42</v>
+      </c>
+      <c r="D20">
+        <v>-2.46</v>
+      </c>
+      <c r="E20">
+        <v>-2.72</v>
+      </c>
+      <c r="F20">
+        <v>-2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>511</v>
+      </c>
+      <c r="B21">
+        <v>-99.426000000000002</v>
+      </c>
+      <c r="C21">
+        <v>-97.992000000000004</v>
+      </c>
+      <c r="D21">
+        <v>-97.28</v>
+      </c>
+      <c r="E21">
+        <v>-96.57</v>
+      </c>
+      <c r="F21">
+        <v>-98.26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>94</v>
+      </c>
+      <c r="B22">
+        <v>-4.6900000000000004</v>
+      </c>
+      <c r="C22">
+        <v>-4.34</v>
+      </c>
+      <c r="D22">
+        <v>-4.04</v>
+      </c>
+      <c r="E22">
+        <v>-3.93</v>
+      </c>
+      <c r="F22">
+        <v>-3.51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>542</v>
+      </c>
+      <c r="B23">
+        <v>-9.68</v>
+      </c>
+      <c r="C23">
+        <v>-10.09</v>
+      </c>
+      <c r="D23">
+        <v>-10.01</v>
+      </c>
+      <c r="E23">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="F23">
+        <v>-10.039999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>166</v>
+      </c>
+      <c r="B24">
+        <v>-5.99</v>
+      </c>
+      <c r="C24">
+        <v>-5.72</v>
+      </c>
+      <c r="D24">
+        <v>-5.29</v>
+      </c>
+      <c r="E24">
+        <v>-5.27</v>
+      </c>
+      <c r="F24">
+        <v>-5.0199999999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>554</v>
+      </c>
+      <c r="B25">
+        <v>-11.18</v>
+      </c>
+      <c r="C25">
+        <v>-11.29</v>
+      </c>
+      <c r="D25">
+        <v>-11.19</v>
+      </c>
+      <c r="E25">
+        <v>-11.55</v>
+      </c>
+      <c r="F25">
+        <v>-11.16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>171</v>
+      </c>
+      <c r="B26">
+        <v>-5.15</v>
+      </c>
+      <c r="C26">
+        <v>-5.7</v>
+      </c>
+      <c r="D26">
+        <v>-5.44</v>
+      </c>
+      <c r="E26">
+        <v>-5.51</v>
+      </c>
+      <c r="F26">
+        <v>-5.34</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>558</v>
+      </c>
+      <c r="B27">
+        <v>-76.242999999999995</v>
+      </c>
+      <c r="C27">
+        <v>-74.808999999999997</v>
+      </c>
+      <c r="D27">
+        <v>-73.98</v>
+      </c>
+      <c r="E27">
+        <v>-73.19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28">
+        <v>-4.34</v>
+      </c>
+      <c r="C28">
+        <v>-4.57</v>
+      </c>
+      <c r="D28">
+        <v>-4.47</v>
+      </c>
+      <c r="E28">
+        <v>-4.5</v>
+      </c>
+      <c r="F28">
+        <v>-4.55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29">
+        <v>-5.42</v>
+      </c>
+      <c r="C29">
+        <v>-4.87</v>
+      </c>
+      <c r="D29">
+        <v>-4.96</v>
+      </c>
+      <c r="E29">
+        <v>-5.05</v>
+      </c>
+      <c r="F29">
+        <v>-5.19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <f>COUNT(B2:B29)</f>
+        <v>28</v>
+      </c>
+      <c r="C30">
+        <f>COUNT(C2:C29)</f>
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <f>COUNT(D2:D29)</f>
+        <v>28</v>
+      </c>
+      <c r="E30">
+        <f>COUNT(E2:E29)</f>
+        <v>27</v>
+      </c>
+      <c r="F30">
+        <f>COUNT(F2:F29)</f>
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -55597,13 +57040,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P514"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A485" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M514" activeCellId="10" sqref="A1:XFD1 C514 D514 E514 G514 H514 I514 J514 K514 L514 M514"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -63887,7 +65330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E514"/>
   <sheetViews>
@@ -68610,7 +70053,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q432"/>
   <sheetViews>
@@ -77203,19 +78646,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView zoomScale="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.1640625" customWidth="1"/>
     <col min="8" max="8" width="11.6640625" customWidth="1"/>
-    <col min="10" max="10" width="14.83203125" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" hidden="1" customWidth="1"/>
     <col min="12" max="12" width="17.83203125" customWidth="1"/>
     <col min="13" max="13" width="46.1640625" customWidth="1"/>
     <col min="14" max="15" width="18.83203125" style="3" customWidth="1"/>
@@ -77245,34 +78688,34 @@
         <v>593</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>625</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>594</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>595</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>596</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>597</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>618</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>619</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B2" s="13">
         <v>0.69493611320516002</v>
@@ -77305,7 +78748,7 @@
         <v>78.36</v>
       </c>
       <c r="M2" s="13" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="N2" s="3">
         <v>1</v>
@@ -77314,12 +78757,12 @@
         <v>1</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B3" s="3">
         <v>0.366741566047593</v>
@@ -77352,7 +78795,7 @@
         <v>10.3</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="N3" s="3">
         <v>1</v>
@@ -77361,12 +78804,12 @@
         <v>1</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="59" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B4" s="3">
         <v>0.27649257911035102</v>
@@ -77399,7 +78842,7 @@
         <v>10.125</v>
       </c>
       <c r="M4" s="16" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="N4" s="3">
         <v>0</v>
@@ -77408,12 +78851,12 @@
         <v>0</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B5" s="3">
         <v>0.16725590663298201</v>
@@ -77446,7 +78889,7 @@
         <v>20.83</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="N5" s="3">
         <v>1</v>
@@ -77455,12 +78898,12 @@
         <v>0</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="6" spans="1:16" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B6" s="3">
         <v>0.232812336577575</v>
@@ -77493,7 +78936,7 @@
         <v>48.826000000000001</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="N6" s="3">
         <v>2</v>
@@ -77502,12 +78945,12 @@
         <v>0</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B7" s="13">
         <v>0.64866218444365498</v>
@@ -77540,7 +78983,7 @@
         <v>20.523</v>
       </c>
       <c r="M7" s="7" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="N7" s="3">
         <v>1</v>
@@ -77549,12 +78992,12 @@
         <v>1</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="62" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B8" s="3">
         <v>0.31691789413965799</v>
@@ -77587,7 +79030,7 @@
         <v>37.219000000000001</v>
       </c>
       <c r="M8" s="18" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="N8" s="3">
         <v>0</v>
@@ -77596,12 +79039,12 @@
         <v>1</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="9" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B9" s="13">
         <v>0.74628172065768705</v>
@@ -77641,12 +79084,12 @@
         <v>1</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B10" s="13">
         <v>0.76114121818119895</v>
@@ -77686,12 +79129,12 @@
         <v>1</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B11" s="3">
         <v>0.41806895920632098</v>
@@ -77731,12 +79174,12 @@
         <v>1</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" s="3" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" s="3" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B12" s="13">
         <v>0.56786769753029698</v>
@@ -77772,12 +79215,12 @@
         <v>1</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="B13" s="13">
         <v>0.68840000000000001</v>
@@ -77813,12 +79256,36 @@
         <v>0</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
-        <v>620</v>
+        <v>619</v>
+      </c>
+      <c r="B14" s="3">
+        <v>0.15717902800928299</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-78.908541509106598</v>
+      </c>
+      <c r="D14" s="3">
+        <v>-2.8548765784997401</v>
+      </c>
+      <c r="E14" s="3">
+        <v>-0.57304010344669598</v>
+      </c>
+      <c r="F14" s="3">
+        <v>7.02644780335436</v>
+      </c>
+      <c r="G14" s="3">
+        <v>-1.05794366942253E-2</v>
+      </c>
+      <c r="H14" s="3">
+        <v>1.9985947097285299</v>
+      </c>
+      <c r="I14" s="3">
+        <v>2.6404000000000001</v>
       </c>
       <c r="K14" s="15">
         <v>34.81</v>
@@ -77832,10 +79299,43 @@
     </row>
     <row r="15" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>625</v>
+        <v>624</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.217341064537203</v>
+      </c>
+      <c r="C15" s="3">
+        <v>-13.0935373797802</v>
+      </c>
+      <c r="D15" s="3">
+        <v>-0.93221239591569305</v>
+      </c>
+      <c r="E15" s="3">
+        <v>-0.60098609760674904</v>
+      </c>
+      <c r="F15" s="3">
+        <v>-1.3330529718265201</v>
+      </c>
+      <c r="G15" s="3">
+        <v>-1.23968054229262E-2</v>
+      </c>
+      <c r="H15" s="3">
+        <v>1.4093124007612601</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1.1341000000000001</v>
+      </c>
+      <c r="K15" s="15">
+        <v>37.78</v>
+      </c>
+      <c r="N15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
+        <v>1</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Fulldata.xls with testsets for Alkanols+water.
</commit_message>
<xml_diff>
--- a/mobley/mnsol/Fulldata.xlsx
+++ b/mobley/mnsol/Fulldata.xlsx
@@ -20,6 +20,7 @@
     <sheet name="Solvents_ions_only" sheetId="4" r:id="rId6"/>
     <sheet name="consistent_set_neutral+ions" sheetId="5" r:id="rId7"/>
     <sheet name="Results" sheetId="6" r:id="rId8"/>
+    <sheet name=" new results" sheetId="10" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13298" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13492" uniqueCount="639">
   <si>
     <t>Compound</t>
   </si>
@@ -1908,10 +1909,49 @@
     <t>Li, Na, K, Cl, Br, I, butanone, ethanol, toluene, 14_dioxane, n_octane, nitromethane</t>
   </si>
   <si>
+    <t>DMA</t>
+  </si>
+  <si>
     <t>Dimethylacetamide</t>
   </si>
   <si>
     <t>B [-2,2]</t>
+  </si>
+  <si>
+    <t>B [-4,4]</t>
+  </si>
+  <si>
+    <t>testset1</t>
+  </si>
+  <si>
+    <t>testset2</t>
+  </si>
+  <si>
+    <t>testset3</t>
+  </si>
+  <si>
+    <t>testset4</t>
+  </si>
+  <si>
+    <t>testset5</t>
+  </si>
+  <si>
+    <t>testset6</t>
+  </si>
+  <si>
+    <t>testset7</t>
+  </si>
+  <si>
+    <t>testset8</t>
+  </si>
+  <si>
+    <t>testset9</t>
+  </si>
+  <si>
+    <t>testset10</t>
+  </si>
+  <si>
+    <t>Li (Rb for but)</t>
   </si>
 </sst>
 </file>
@@ -2051,7 +2091,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2096,6 +2136,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2799,6 +2842,451 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1086757</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>431800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10007600" y="254000"/>
+          <a:ext cx="807357" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>56777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1003300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>758120</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10096500" y="2736477"/>
+          <a:ext cx="635000" cy="701343"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>42454</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>685800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10121900" y="1998254"/>
+          <a:ext cx="625475" cy="643346"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>81430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1082375</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>830730</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10033000" y="4120030"/>
+          <a:ext cx="777575" cy="749300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>126253</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1320800</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>450051</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9804400" y="6133353"/>
+          <a:ext cx="1244600" cy="323798"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>80683</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1300046</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>499783</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9842500" y="5528983"/>
+          <a:ext cx="1185746" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>50800</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>105462</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1358900</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>466911</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9779000" y="4994962"/>
+          <a:ext cx="1308100" cy="361449"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>110647</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1371600</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>442258</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9766300" y="3590447"/>
+          <a:ext cx="1333500" cy="331611"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>42093</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1168400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>713442</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9969500" y="1273993"/>
+          <a:ext cx="927100" cy="671349"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>121771</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>1338416</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>439271</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9817100" y="794871"/>
+          <a:ext cx="1249516" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -56419,18 +56907,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="8" max="17" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -56449,8 +56938,38 @@
       <c r="F1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>628</v>
+      </c>
+      <c r="I1" t="s">
+        <v>629</v>
+      </c>
+      <c r="J1" t="s">
+        <v>630</v>
+      </c>
+      <c r="K1" t="s">
+        <v>631</v>
+      </c>
+      <c r="L1" t="s">
+        <v>632</v>
+      </c>
+      <c r="M1" t="s">
+        <v>633</v>
+      </c>
+      <c r="N1" t="s">
+        <v>634</v>
+      </c>
+      <c r="O1" t="s">
+        <v>635</v>
+      </c>
+      <c r="P1" t="s">
+        <v>636</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>329</v>
       </c>
@@ -56469,8 +56988,38 @@
       <c r="F2">
         <v>-11.35</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>346</v>
+      </c>
+      <c r="I2" t="s">
+        <v>346</v>
+      </c>
+      <c r="J2" t="s">
+        <v>346</v>
+      </c>
+      <c r="K2" t="s">
+        <v>346</v>
+      </c>
+      <c r="L2" t="s">
+        <v>346</v>
+      </c>
+      <c r="M2" t="s">
+        <v>346</v>
+      </c>
+      <c r="N2" t="s">
+        <v>346</v>
+      </c>
+      <c r="O2" t="s">
+        <v>346</v>
+      </c>
+      <c r="P2" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>336</v>
       </c>
@@ -56489,8 +57038,38 @@
       <c r="F3">
         <v>-10.47</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>361</v>
+      </c>
+      <c r="I3" t="s">
+        <v>361</v>
+      </c>
+      <c r="J3" t="s">
+        <v>361</v>
+      </c>
+      <c r="K3" t="s">
+        <v>361</v>
+      </c>
+      <c r="L3" t="s">
+        <v>361</v>
+      </c>
+      <c r="M3" t="s">
+        <v>361</v>
+      </c>
+      <c r="N3" t="s">
+        <v>361</v>
+      </c>
+      <c r="O3" t="s">
+        <v>361</v>
+      </c>
+      <c r="P3" t="s">
+        <v>361</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>88</v>
       </c>
@@ -56509,8 +57088,38 @@
       <c r="F4">
         <v>-3.72</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>362</v>
+      </c>
+      <c r="I4" t="s">
+        <v>362</v>
+      </c>
+      <c r="J4" t="s">
+        <v>362</v>
+      </c>
+      <c r="K4" t="s">
+        <v>362</v>
+      </c>
+      <c r="L4" t="s">
+        <v>362</v>
+      </c>
+      <c r="M4" t="s">
+        <v>362</v>
+      </c>
+      <c r="N4" t="s">
+        <v>362</v>
+      </c>
+      <c r="O4" t="s">
+        <v>362</v>
+      </c>
+      <c r="P4" t="s">
+        <v>362</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>346</v>
       </c>
@@ -56529,8 +57138,38 @@
       <c r="F5">
         <v>-62.61</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>446</v>
+      </c>
+      <c r="I5" t="s">
+        <v>446</v>
+      </c>
+      <c r="J5" t="s">
+        <v>446</v>
+      </c>
+      <c r="K5" t="s">
+        <v>446</v>
+      </c>
+      <c r="L5" t="s">
+        <v>446</v>
+      </c>
+      <c r="M5" t="s">
+        <v>446</v>
+      </c>
+      <c r="N5" t="s">
+        <v>446</v>
+      </c>
+      <c r="O5" t="s">
+        <v>446</v>
+      </c>
+      <c r="P5" t="s">
+        <v>446</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>106</v>
       </c>
@@ -56549,8 +57188,38 @@
       <c r="F6">
         <v>-5.71</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>638</v>
+      </c>
+      <c r="I6" t="s">
+        <v>638</v>
+      </c>
+      <c r="J6" t="s">
+        <v>638</v>
+      </c>
+      <c r="K6" t="s">
+        <v>638</v>
+      </c>
+      <c r="L6" t="s">
+        <v>638</v>
+      </c>
+      <c r="M6" t="s">
+        <v>638</v>
+      </c>
+      <c r="N6" t="s">
+        <v>638</v>
+      </c>
+      <c r="O6" t="s">
+        <v>638</v>
+      </c>
+      <c r="P6" t="s">
+        <v>638</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>57</v>
       </c>
@@ -56569,8 +57238,38 @@
       <c r="F7">
         <v>-3.78</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>511</v>
+      </c>
+      <c r="I7" t="s">
+        <v>511</v>
+      </c>
+      <c r="J7" t="s">
+        <v>511</v>
+      </c>
+      <c r="K7" t="s">
+        <v>511</v>
+      </c>
+      <c r="L7" t="s">
+        <v>511</v>
+      </c>
+      <c r="M7" t="s">
+        <v>511</v>
+      </c>
+      <c r="N7" t="s">
+        <v>511</v>
+      </c>
+      <c r="O7" t="s">
+        <v>511</v>
+      </c>
+      <c r="P7" t="s">
+        <v>511</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>361</v>
       </c>
@@ -56589,8 +57288,38 @@
       <c r="F8">
         <v>-68.19</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>329</v>
+      </c>
+      <c r="I8" t="s">
+        <v>336</v>
+      </c>
+      <c r="J8" t="s">
+        <v>336</v>
+      </c>
+      <c r="K8" t="s">
+        <v>88</v>
+      </c>
+      <c r="L8" t="s">
+        <v>336</v>
+      </c>
+      <c r="M8" t="s">
+        <v>329</v>
+      </c>
+      <c r="N8" t="s">
+        <v>329</v>
+      </c>
+      <c r="O8" t="s">
+        <v>329</v>
+      </c>
+      <c r="P8" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>362</v>
       </c>
@@ -56606,8 +57335,38 @@
       <c r="E9">
         <v>-68.67</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L9" t="s">
+        <v>77</v>
+      </c>
+      <c r="M9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" t="s">
+        <v>84</v>
+      </c>
+      <c r="O9" t="s">
+        <v>336</v>
+      </c>
+      <c r="P9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>84</v>
       </c>
@@ -56626,8 +57385,38 @@
       <c r="F10">
         <v>-3.46</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" t="s">
+        <v>405</v>
+      </c>
+      <c r="J10" t="s">
+        <v>405</v>
+      </c>
+      <c r="K10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" t="s">
+        <v>76</v>
+      </c>
+      <c r="M10" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" t="s">
+        <v>77</v>
+      </c>
+      <c r="O10" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10" t="s">
+        <v>84</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>405</v>
       </c>
@@ -56646,8 +57435,38 @@
       <c r="F11">
         <v>-0.64</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K11" t="s">
+        <v>77</v>
+      </c>
+      <c r="L11" t="s">
+        <v>485</v>
+      </c>
+      <c r="M11" t="s">
+        <v>84</v>
+      </c>
+      <c r="N11" t="s">
+        <v>76</v>
+      </c>
+      <c r="O11" t="s">
+        <v>542</v>
+      </c>
+      <c r="P11" t="s">
+        <v>405</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>77</v>
       </c>
@@ -56666,8 +57485,38 @@
       <c r="F12">
         <v>-4.3600000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>487</v>
+      </c>
+      <c r="I12" t="s">
+        <v>479</v>
+      </c>
+      <c r="J12" t="s">
+        <v>499</v>
+      </c>
+      <c r="K12" t="s">
+        <v>145</v>
+      </c>
+      <c r="L12" t="s">
+        <v>499</v>
+      </c>
+      <c r="M12" t="s">
+        <v>76</v>
+      </c>
+      <c r="N12" t="s">
+        <v>94</v>
+      </c>
+      <c r="O12" t="s">
+        <v>166</v>
+      </c>
+      <c r="P12" t="s">
+        <v>479</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>446</v>
       </c>
@@ -56686,8 +57535,38 @@
       <c r="F13">
         <v>-80.930000000000007</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>542</v>
+      </c>
+      <c r="I13" t="s">
+        <v>94</v>
+      </c>
+      <c r="J13" t="s">
+        <v>542</v>
+      </c>
+      <c r="K13" t="s">
+        <v>166</v>
+      </c>
+      <c r="L13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M13" t="s">
+        <v>145</v>
+      </c>
+      <c r="N13" t="s">
+        <v>542</v>
+      </c>
+      <c r="O13" t="s">
+        <v>554</v>
+      </c>
+      <c r="P13" t="s">
+        <v>485</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>447</v>
       </c>
@@ -56703,8 +57582,38 @@
       <c r="F14">
         <v>-123.89</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>171</v>
+      </c>
+      <c r="I14" t="s">
+        <v>166</v>
+      </c>
+      <c r="J14" t="s">
+        <v>554</v>
+      </c>
+      <c r="K14" t="s">
+        <v>554</v>
+      </c>
+      <c r="L14" t="s">
+        <v>542</v>
+      </c>
+      <c r="M14" t="s">
+        <v>554</v>
+      </c>
+      <c r="N14" t="s">
+        <v>71</v>
+      </c>
+      <c r="O14" t="s">
+        <v>171</v>
+      </c>
+      <c r="P14" t="s">
+        <v>487</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>76</v>
       </c>
@@ -56723,8 +57632,38 @@
       <c r="F15">
         <v>-3.87</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" t="s">
+        <v>4</v>
+      </c>
+      <c r="K15" t="s">
+        <v>71</v>
+      </c>
+      <c r="L15" t="s">
+        <v>171</v>
+      </c>
+      <c r="M15" t="s">
+        <v>4</v>
+      </c>
+      <c r="N15" t="s">
+        <v>4</v>
+      </c>
+      <c r="O15" t="s">
+        <v>4</v>
+      </c>
+      <c r="P15" t="s">
+        <v>499</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>479</v>
       </c>
@@ -78651,7 +79590,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView zoomScale="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:L8"/>
+      <selection sqref="A1:P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -78688,7 +79627,7 @@
         <v>593</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>594</v>
@@ -79299,7 +80238,7 @@
     </row>
     <row r="15" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="B15" s="3">
         <v>0.217341064537203</v>
@@ -79336,6 +80275,571 @@
       </c>
       <c r="P15" s="2" t="s">
         <v>623</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="19.33203125" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" customWidth="1"/>
+    <col min="13" max="13" width="46.1640625" customWidth="1"/>
+    <col min="16" max="16" width="36.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>589</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>627</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>595</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>596</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>613</v>
+      </c>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3" t="s">
+        <v>617</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>618</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="37" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>597</v>
+      </c>
+      <c r="B2" s="13">
+        <v>0.65979935317407901</v>
+      </c>
+      <c r="C2" s="5">
+        <v>-30.716953215161301</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.112703436122278</v>
+      </c>
+      <c r="E2" s="5">
+        <v>-8.3097117217093203E-2</v>
+      </c>
+      <c r="F2" s="5">
+        <v>-0.16227801116082499</v>
+      </c>
+      <c r="G2" s="5">
+        <v>4.7804767517177597E-3</v>
+      </c>
+      <c r="H2" s="5">
+        <v>1.06129266287354</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1.6</v>
+      </c>
+      <c r="J2" s="5">
+        <v>1.85</v>
+      </c>
+      <c r="K2" s="20">
+        <v>78.36</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>598</v>
+      </c>
+      <c r="N2" s="3">
+        <v>1</v>
+      </c>
+      <c r="O2" s="3">
+        <v>1</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>599</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.40048430415499398</v>
+      </c>
+      <c r="C3" s="5">
+        <v>-27.4264166862617</v>
+      </c>
+      <c r="D3" s="5">
+        <v>-0.17675337014966699</v>
+      </c>
+      <c r="E3" s="5">
+        <v>-0.108374675747628</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.90372296636461902</v>
+      </c>
+      <c r="G3" s="5">
+        <v>-1.7196666049524599E-2</v>
+      </c>
+      <c r="H3" s="5">
+        <v>3.8887636175368998</v>
+      </c>
+      <c r="I3" s="5">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="J3" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="K3" s="20">
+        <v>10.3</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="3">
+        <v>1</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.35929425867980302</v>
+      </c>
+      <c r="C4" s="5">
+        <v>-93.318068312098106</v>
+      </c>
+      <c r="D4" s="5">
+        <v>-1.0403956724438299</v>
+      </c>
+      <c r="E4" s="5">
+        <v>-0.31073343163058598</v>
+      </c>
+      <c r="F4" s="5">
+        <v>-3.7962305963829301</v>
+      </c>
+      <c r="G4" s="5">
+        <v>-2.01504596964002E-2</v>
+      </c>
+      <c r="H4" s="5">
+        <v>3.99936300691017</v>
+      </c>
+      <c r="I4" s="5">
+        <v>2.9872999999999998</v>
+      </c>
+      <c r="J4" s="5">
+        <v>1.83</v>
+      </c>
+      <c r="K4" s="20">
+        <v>10.125</v>
+      </c>
+      <c r="M4" s="16" t="s">
+        <v>602</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>0</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="57" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>603</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.53937947692043797</v>
+      </c>
+      <c r="C5" s="5">
+        <v>-9.33708945496317</v>
+      </c>
+      <c r="D5" s="5">
+        <v>-0.10800786005287</v>
+      </c>
+      <c r="E5" s="5">
+        <v>-0.38125620743183503</v>
+      </c>
+      <c r="F5" s="5">
+        <v>-0.72863758962456504</v>
+      </c>
+      <c r="G5" s="5">
+        <v>-2.2285590183705802E-2</v>
+      </c>
+      <c r="H5" s="5">
+        <v>3.9658457167217001</v>
+      </c>
+      <c r="I5" s="5">
+        <v>1.1317999999999999</v>
+      </c>
+      <c r="J5" s="5">
+        <v>2.88</v>
+      </c>
+      <c r="K5" s="20">
+        <v>20.83</v>
+      </c>
+      <c r="M5" s="14" t="s">
+        <v>604</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.490307640063885</v>
+      </c>
+      <c r="C6" s="5">
+        <v>-11.523762468931</v>
+      </c>
+      <c r="D6" s="5">
+        <v>-0.31993531324417301</v>
+      </c>
+      <c r="E6" s="5">
+        <v>-0.380190336689467</v>
+      </c>
+      <c r="F6" s="5">
+        <v>-0.25214739323076801</v>
+      </c>
+      <c r="G6" s="5">
+        <v>-1.9170629778025399E-2</v>
+      </c>
+      <c r="H6" s="5">
+        <v>3.9261329599710999</v>
+      </c>
+      <c r="I6" s="5">
+        <v>1.3627</v>
+      </c>
+      <c r="J6" s="5">
+        <v>3.96</v>
+      </c>
+      <c r="K6" s="20">
+        <v>48.826000000000001</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>606</v>
+      </c>
+      <c r="N6" s="3">
+        <v>2</v>
+      </c>
+      <c r="O6" s="3">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>607</v>
+      </c>
+      <c r="B7" s="13">
+        <v>0.68804933936335499</v>
+      </c>
+      <c r="C7" s="5">
+        <v>-31.6267637992412</v>
+      </c>
+      <c r="D7" s="5">
+        <v>0.38783429295079502</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1.5608840643882601E-2</v>
+      </c>
+      <c r="F7" s="5">
+        <v>-0.56248007345113704</v>
+      </c>
+      <c r="G7" s="5">
+        <v>-1.7456291948014301E-2</v>
+      </c>
+      <c r="H7" s="5">
+        <v>3.3343400515600701</v>
+      </c>
+      <c r="I7" s="5">
+        <v>1.7070000000000001</v>
+      </c>
+      <c r="J7" s="5">
+        <v>1.68</v>
+      </c>
+      <c r="K7" s="20">
+        <v>20.523</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>608</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1</v>
+      </c>
+      <c r="O7" s="3">
+        <v>1</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="67" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>609</v>
+      </c>
+      <c r="B8" s="5">
+        <v>0.39131803526671399</v>
+      </c>
+      <c r="C8" s="5">
+        <v>-87.874670486271597</v>
+      </c>
+      <c r="D8" s="5">
+        <v>0.58838936640790096</v>
+      </c>
+      <c r="E8" s="5">
+        <v>-0.190490664469608</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.16521714216728001</v>
+      </c>
+      <c r="G8" s="5">
+        <v>-1.5783033855283998E-2</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2.4019352564193799</v>
+      </c>
+      <c r="I8" s="5">
+        <v>1.6659999999999999</v>
+      </c>
+      <c r="J8" s="5">
+        <v>3.82</v>
+      </c>
+      <c r="K8" s="20">
+        <v>37.219000000000001</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>615</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>1</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>610</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0.66452512999722002</v>
+      </c>
+      <c r="C9" s="5">
+        <v>-11.8739116174467</v>
+      </c>
+      <c r="D9" s="5">
+        <v>0.262442338600681</v>
+      </c>
+      <c r="E9" s="5">
+        <v>-7.71821479897596E-2</v>
+      </c>
+      <c r="F9" s="5">
+        <v>3.0149565289015099</v>
+      </c>
+      <c r="G9" s="5">
+        <v>-2.0002783540631001E-2</v>
+      </c>
+      <c r="H9" s="5">
+        <v>3.9964429781321398</v>
+      </c>
+      <c r="I9" s="5">
+        <v>1.4233</v>
+      </c>
+      <c r="J9" s="5">
+        <v>1.69</v>
+      </c>
+      <c r="K9" s="20">
+        <v>24.852</v>
+      </c>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3">
+        <v>1</v>
+      </c>
+      <c r="O9" s="3">
+        <v>1</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>611</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.66568497101240198</v>
+      </c>
+      <c r="C10" s="5">
+        <v>-12.480776559776199</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.23611407097728199</v>
+      </c>
+      <c r="E10" s="5">
+        <v>-5.7096305800275499E-2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3.2378004861702698</v>
+      </c>
+      <c r="G10" s="5">
+        <v>-1.9460038514259499E-2</v>
+      </c>
+      <c r="H10" s="5">
+        <v>3.9827876712230199</v>
+      </c>
+      <c r="I10" s="5">
+        <v>1.7729999999999999</v>
+      </c>
+      <c r="J10" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="K10" s="20">
+        <v>32.613</v>
+      </c>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3">
+        <v>1</v>
+      </c>
+      <c r="O10" s="3">
+        <v>1</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="44" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>612</v>
+      </c>
+      <c r="B11" s="5">
+        <v>0.66267288113971201</v>
+      </c>
+      <c r="C11" s="5">
+        <v>-9.7690460751389203</v>
+      </c>
+      <c r="D11" s="5">
+        <v>9.0010393395208804E-2</v>
+      </c>
+      <c r="E11" s="5">
+        <v>-0.33956536444269703</v>
+      </c>
+      <c r="F11" s="5">
+        <v>1.08305064676924</v>
+      </c>
+      <c r="G11" s="5">
+        <v>-1.74229547845644E-2</v>
+      </c>
+      <c r="H11" s="5">
+        <v>2.7674361087696302</v>
+      </c>
+      <c r="I11" s="5">
+        <v>1.266</v>
+      </c>
+      <c r="J11" s="5">
+        <v>3.92</v>
+      </c>
+      <c r="K11" s="20">
+        <v>35.688000000000002</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3">
+        <v>1</v>
+      </c>
+      <c r="O11" s="3">
+        <v>1</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>624</v>
+      </c>
+      <c r="B13">
+        <v>0.217341064537203</v>
+      </c>
+      <c r="C13">
+        <v>-13.0935373797802</v>
+      </c>
+      <c r="D13">
+        <v>-0.93221239591569305</v>
+      </c>
+      <c r="E13">
+        <v>-0.60098609760674904</v>
+      </c>
+      <c r="F13">
+        <v>-1.3330529718265201</v>
+      </c>
+      <c r="G13">
+        <v>-1.23968054229262E-2</v>
+      </c>
+      <c r="H13">
+        <v>1.4093124007612601</v>
       </c>
     </row>
   </sheetData>

</xml_diff>